<commit_message>
Y2A - MS Teams Assignment Update: Learning Log + Assessment Rubric
</commit_message>
<xml_diff>
--- a/docs/Year2/BlockA/MS Teams Assignment Template/2022-23 ADS&AI Assessment Rubric Y2A.xlsx
+++ b/docs/Year2/BlockA/MS Teams Assignment Template/2022-23 ADS&AI Assessment Rubric Y2A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bramh\Documents\GitHub\AAI-DM\docs\Year2\BlockA\MS Teams Assignment Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6398EDE6-DE50-45C1-B510-FD02EDD6CA66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A8EE8B-B913-4B92-9660-E44E3AD53F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="50910" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="208">
   <si>
     <t>Student Self-Assessment</t>
   </si>
@@ -219,9 +219,6 @@
   </si>
   <si>
     <t xml:space="preserve">All references to important resources used are included. Your evidence is clear and to the point. And meeting all criteria in sufficient. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your writing style is professional and free of spelling and grammar mistakes. Clear what was done and why given individual and project feedback. And meeting all criteria in good. </t>
   </si>
   <si>
     <t>1,2</t>
@@ -289,13 +286,7 @@
     <t>Appropriate qualitative methods (e.g., interviews) are chosen and their motivation is documented by means of a clear purpose statement..  And meeting all criteria in poor.</t>
   </si>
   <si>
-    <t>The study design is documented in the research proposal.And meeting all criteria in insufficient.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Individual contribution to quantitative and qualitative data collection is clearly documented. And meeting all criteria in sufficient. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Student is able to design a reliable and valid scale and use integrate data collected using the designed scale with qualitative data by choosing appropriate mixed methods. And meeting all criteria in good. </t>
   </si>
   <si>
     <t>3, 11</t>
@@ -368,12 +359,6 @@
     <t xml:space="preserve">The student proposes clear decisions based on the collected evidence and quantifies uncertainity where necessary. To increase our confidence in the proposed decision, power analyses was carried out and interpreted correctly. And meeting all criteria in good. </t>
   </si>
   <si>
-    <t>6.0 Scientific Reporting: The student is able to communicate findings by means of a structured, coherent, and well argued  scientific report using Latex</t>
-  </si>
-  <si>
-    <t>The student is able to communicate findings by means of a structured, coherent, and well argued  scientific report using Latex</t>
-  </si>
-  <si>
     <t>A literature review is present and appropriate sources of are used. Latex is used for drafting the document.</t>
   </si>
   <si>
@@ -431,9 +416,6 @@
     <t>Problem analysis</t>
   </si>
   <si>
-    <t>The student cn analyse a problem by describing the context, trade-offs and formulation of the final demand (as a result of a process of demand articulation). In doing so, The student identifies the possible solutions. As a result, The student can formulate an approach for a data trajectory considering relevant actors and interests, involving relevant theories and (technical) possibilities.</t>
-  </si>
-  <si>
     <t>Domain knowledge</t>
   </si>
   <si>
@@ -455,19 +437,10 @@
     <t>Data analysis</t>
   </si>
   <si>
-    <t>The studentan can use analytical and statistical methods to analyse data to create value for individuals, organizations and domains.</t>
-  </si>
-  <si>
     <t>Modelling</t>
   </si>
   <si>
-    <t>The studentan apply modelling techniques including Machine Learning and AI to create value for individuals, organizations and domains.</t>
-  </si>
-  <si>
     <t>Design, prototyping and implementation</t>
-  </si>
-  <si>
-    <t>The studentan develop a prototype using an iterative cycle, explicitly involving stakeholders, and implement applications within an (existing) architecture.</t>
   </si>
   <si>
     <t>Evaluation &amp; Deployment</t>
@@ -543,33 +516,6 @@
   </si>
   <si>
     <t>Have the learning skills to allow them to continue to study in a manner that may be largely self-directed or autonomous.</t>
-  </si>
-  <si>
-    <t>BLOCK C</t>
-  </si>
-  <si>
-    <t>Knowledge &amp; Insight</t>
-  </si>
-  <si>
-    <t>Application of K&amp;I</t>
-  </si>
-  <si>
-    <t>Can apply modelling techniques including Machine Learning and AI to create value for individuals, organizations and domains.</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>Can develop a prototype using an iterative cycle, explicitly involving stakeholders, and implement applications within an (existing) architecture.</t>
-  </si>
-  <si>
-    <t>Can collaborate (internationally) in multidisciplinary teams with different levels of knowledge in the field of data use and applications. She can set up and execute projects in collaboration with stakeholders and team members. She can act as a sounding board in discussions with team members, customers, users and experts. She strives for a good balance between input of her own vision and additional expertise of others. She is able to lead a team.</t>
-  </si>
-  <si>
-    <t>Applies relevant (research) methods and techniques in combination with relevant and adequate argumentation. She can reflect on (business) processes and her role in them, both theoretically and practically, by constantly evaluating her own actions and adapting them with input from others. She can translate the result of the reflection into concrete personal learning objectives.</t>
-  </si>
-  <si>
-    <t>Is aware of legal and ethical aspects within the context of her professional work environment and is able to make substantiated considerations in this regard. She acts from justice and integrity.</t>
   </si>
   <si>
     <t>ILO</t>
@@ -811,13 +757,59 @@
   </si>
   <si>
     <t xml:space="preserve">Student shows clear understanding of the purpose of each of the documents. Submissions are at a professional level with regards to language used, writing styles, content and tidiness. And meeting all criteria in good. </t>
+  </si>
+  <si>
+    <t>PROJECT TOTAL</t>
+  </si>
+  <si>
+    <t>YOUR TOTAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your writing style is professional and free of spelling and grammar mistakes. Feedback is taken into account and is acted upon. And meeting all criteria in good. </t>
+  </si>
+  <si>
+    <t>The study design is documented in the research proposal. And meeting all criteria in insufficient.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Student is able to report on the reliability and validity of the chosen instrument and  integrate data collected using the instrument with qualitative data by choosing appropriate mixed methods. And meeting all criteria in good. </t>
+  </si>
+  <si>
+    <t>Competencies</t>
+  </si>
+  <si>
+    <t>The student can use analytical and statistical methods to analyse data to create value for individuals, organizations and domains.</t>
+  </si>
+  <si>
+    <t>The student can apply modelling techniques including Machine Learning and AI to create value for individuals, organizations and domains.</t>
+  </si>
+  <si>
+    <t>The student can develop a prototype using an iterative cycle, explicitly involving stakeholders, and implement applications within an (existing) architecture.</t>
+  </si>
+  <si>
+    <t>The student can analyse a problem by describing the context, trade-offs and formulation of the final demand (as a result of a process of demand articulation). In doing so, The student identifies the possible solutions. As a result, The student can formulate an approach for a data trajectory considering relevant actors and interests, involving relevant theories and (technical) possibilities.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">6.0 Scientific Reporting: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">The student is able to communicate findings by means of a structured, coherent, and well argued  scientific report using Latex. </t>
+    </r>
+  </si>
+  <si>
+    <t>The student is able to communicate findings by means of a structured, coherent, and well argued  scientific report using Latex.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -954,35 +946,9 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="20"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -1003,8 +969,22 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="52">
+  <fills count="50">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1163,12 +1143,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFE1CC"/>
         <bgColor rgb="FFFCE5CD"/>
       </patternFill>
@@ -1283,24 +1257,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor rgb="FFCFE2F3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFBDAD7"/>
         <bgColor rgb="FFF4CCCC"/>
       </patternFill>
@@ -1311,19 +1267,20 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="3">
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
       <right/>
       <top/>
       <bottom/>
@@ -1333,55 +1290,6 @@
       <left/>
       <right style="thin">
         <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
@@ -1398,148 +1306,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="185">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1667,6 +1441,9 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1679,9 +1456,6 @@
     <xf numFmtId="0" fontId="7" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1692,6 +1466,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1704,14 +1481,17 @@
     <xf numFmtId="0" fontId="1" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1720,16 +1500,16 @@
     <xf numFmtId="0" fontId="7" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1738,87 +1518,18 @@
     <xf numFmtId="0" fontId="7" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="47" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="47" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="48" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="49" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="49" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="50" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1827,8 +1538,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1837,18 +1548,15 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1859,6 +1567,8 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="48" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="27" fillId="49" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1876,41 +1586,41 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1959,19 +1669,19 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1980,52 +1690,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2036,7 +1714,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{9902F182-0AFB-1F41-B571-EB1D4AC04E32}"/>
   </cellStyles>
@@ -2584,16 +2264,16 @@
   </sheetPr>
   <dimension ref="A1:W54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26:E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="39" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="39" customWidth="1"/>
-    <col min="3" max="3" width="5.42578125" style="39" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="39" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" style="39" customWidth="1"/>
     <col min="5" max="5" width="22.85546875" style="39" customWidth="1"/>
     <col min="6" max="6" width="27.42578125" style="39" customWidth="1"/>
@@ -2628,11 +2308,11 @@
     <row r="2" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="17"/>
       <c r="B2" s="18"/>
-      <c r="C2" s="124" t="s">
+      <c r="C2" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="125"/>
-      <c r="E2" s="125"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
@@ -2648,8 +2328,8 @@
     <row r="3" spans="1:16" s="23" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="19"/>
       <c r="B3" s="20"/>
-      <c r="C3" s="143"/>
-      <c r="D3" s="144"/>
+      <c r="C3" s="121"/>
+      <c r="D3" s="122"/>
       <c r="E3" s="38" t="s">
         <v>1</v>
       </c>
@@ -2659,40 +2339,40 @@
       <c r="G3" s="21"/>
       <c r="H3" s="22"/>
       <c r="I3" s="22"/>
-      <c r="J3" s="127" t="s">
+      <c r="J3" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="145"/>
-      <c r="L3" s="146" t="s">
+      <c r="K3" s="123"/>
+      <c r="L3" s="124" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="125"/>
-      <c r="N3" s="125"/>
+      <c r="M3" s="103"/>
+      <c r="N3" s="103"/>
       <c r="O3" s="20"/>
       <c r="P3" s="19"/>
     </row>
     <row r="4" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17"/>
       <c r="B4" s="24"/>
-      <c r="C4" s="147" t="s">
+      <c r="C4" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="125"/>
+      <c r="D4" s="103"/>
       <c r="E4" s="15"/>
-      <c r="F4" s="148"/>
-      <c r="G4" s="149"/>
-      <c r="H4" s="149"/>
-      <c r="I4" s="149"/>
-      <c r="J4" s="150"/>
-      <c r="K4" s="151"/>
-      <c r="L4" s="152" t="s">
+      <c r="F4" s="126"/>
+      <c r="G4" s="127"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="128"/>
+      <c r="K4" s="129"/>
+      <c r="L4" s="130" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="153">
+      <c r="M4" s="131">
         <f>IF(ROUND((N24/10),1)&lt;&gt;ROUND((N24/10),0),ROUND((N2/10),1),ROUND((N24/10),0))</f>
         <v>0</v>
       </c>
-      <c r="N4" s="154" t="str">
+      <c r="N4" s="132" t="str">
         <f>IF(M4&gt;=5.5,"PASS",IF(M4&gt;0,"FAIL","M/O"))</f>
         <v>M/O</v>
       </c>
@@ -2702,86 +2382,86 @@
     <row r="5" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="17"/>
       <c r="B5" s="24"/>
-      <c r="C5" s="147" t="s">
+      <c r="C5" s="125" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="145"/>
+      <c r="D5" s="123"/>
       <c r="E5" s="15"/>
-      <c r="F5" s="149"/>
-      <c r="G5" s="149"/>
-      <c r="H5" s="149"/>
-      <c r="I5" s="149"/>
-      <c r="J5" s="151"/>
-      <c r="K5" s="151"/>
-      <c r="L5" s="145"/>
-      <c r="M5" s="145"/>
-      <c r="N5" s="145"/>
+      <c r="F5" s="127"/>
+      <c r="G5" s="127"/>
+      <c r="H5" s="127"/>
+      <c r="I5" s="127"/>
+      <c r="J5" s="129"/>
+      <c r="K5" s="129"/>
+      <c r="L5" s="123"/>
+      <c r="M5" s="123"/>
+      <c r="N5" s="123"/>
       <c r="O5" s="18"/>
       <c r="P5" s="17"/>
     </row>
     <row r="6" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="17"/>
       <c r="B6" s="24"/>
-      <c r="C6" s="147" t="s">
+      <c r="C6" s="125" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="155"/>
-      <c r="E6" s="120" t="s">
+      <c r="D6" s="133"/>
+      <c r="E6" s="96" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="149"/>
-      <c r="G6" s="149"/>
-      <c r="H6" s="149"/>
-      <c r="I6" s="149"/>
-      <c r="J6" s="151"/>
-      <c r="K6" s="151"/>
-      <c r="L6" s="145"/>
-      <c r="M6" s="145"/>
-      <c r="N6" s="145"/>
+      <c r="F6" s="127"/>
+      <c r="G6" s="127"/>
+      <c r="H6" s="127"/>
+      <c r="I6" s="127"/>
+      <c r="J6" s="129"/>
+      <c r="K6" s="129"/>
+      <c r="L6" s="123"/>
+      <c r="M6" s="123"/>
+      <c r="N6" s="123"/>
       <c r="O6" s="18"/>
       <c r="P6" s="17"/>
     </row>
     <row r="7" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="17"/>
       <c r="B7" s="24"/>
-      <c r="C7" s="147" t="s">
+      <c r="C7" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="145"/>
+      <c r="D7" s="123"/>
       <c r="E7" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="149"/>
-      <c r="G7" s="149"/>
-      <c r="H7" s="149"/>
-      <c r="I7" s="149"/>
-      <c r="J7" s="151"/>
-      <c r="K7" s="151"/>
-      <c r="L7" s="145"/>
-      <c r="M7" s="145"/>
-      <c r="N7" s="145"/>
+      <c r="F7" s="127"/>
+      <c r="G7" s="127"/>
+      <c r="H7" s="127"/>
+      <c r="I7" s="127"/>
+      <c r="J7" s="129"/>
+      <c r="K7" s="129"/>
+      <c r="L7" s="123"/>
+      <c r="M7" s="123"/>
+      <c r="N7" s="123"/>
       <c r="O7" s="18"/>
       <c r="P7" s="17"/>
     </row>
     <row r="8" spans="1:16" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17"/>
       <c r="B8" s="24"/>
-      <c r="C8" s="156" t="s">
+      <c r="C8" s="134" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="157"/>
+      <c r="D8" s="135"/>
       <c r="E8" s="40" t="s">
-        <v>212</v>
-      </c>
-      <c r="F8" s="149"/>
-      <c r="G8" s="149"/>
-      <c r="H8" s="149"/>
-      <c r="I8" s="149"/>
-      <c r="J8" s="151"/>
-      <c r="K8" s="151"/>
-      <c r="L8" s="145"/>
-      <c r="M8" s="145"/>
-      <c r="N8" s="145"/>
+        <v>194</v>
+      </c>
+      <c r="F8" s="127"/>
+      <c r="G8" s="127"/>
+      <c r="H8" s="127"/>
+      <c r="I8" s="127"/>
+      <c r="J8" s="129"/>
+      <c r="K8" s="129"/>
+      <c r="L8" s="123"/>
+      <c r="M8" s="123"/>
+      <c r="N8" s="123"/>
       <c r="O8" s="18"/>
       <c r="P8" s="17"/>
     </row>
@@ -2824,11 +2504,11 @@
     <row r="11" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A11" s="17"/>
       <c r="B11" s="18"/>
-      <c r="C11" s="124" t="s">
+      <c r="C11" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="125"/>
-      <c r="E11" s="125"/>
+      <c r="D11" s="103"/>
+      <c r="E11" s="103"/>
       <c r="F11" s="18"/>
       <c r="G11" s="18"/>
       <c r="H11" s="18"/>
@@ -2844,7 +2524,9 @@
     <row r="12" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="17"/>
       <c r="B12" s="18"/>
-      <c r="C12" s="43"/>
+      <c r="C12" s="43" t="s">
+        <v>201</v>
+      </c>
       <c r="D12" s="44" t="s">
         <v>14</v>
       </c>
@@ -2882,34 +2564,34 @@
     <row r="13" spans="1:16" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="17"/>
       <c r="B13" s="27"/>
-      <c r="C13" s="158">
+      <c r="C13" s="136">
         <v>9</v>
       </c>
-      <c r="D13" s="166" t="s">
+      <c r="D13" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="166"/>
-      <c r="F13" s="166"/>
-      <c r="G13" s="166"/>
-      <c r="H13" s="166"/>
-      <c r="I13" s="166"/>
-      <c r="J13" s="166"/>
-      <c r="K13" s="166"/>
-      <c r="L13" s="105"/>
-      <c r="M13" s="105"/>
-      <c r="N13" s="105"/>
+      <c r="E13" s="144"/>
+      <c r="F13" s="144"/>
+      <c r="G13" s="144"/>
+      <c r="H13" s="144"/>
+      <c r="I13" s="144"/>
+      <c r="J13" s="144"/>
+      <c r="K13" s="144"/>
+      <c r="L13" s="82"/>
+      <c r="M13" s="82"/>
+      <c r="N13" s="82"/>
       <c r="O13" s="28"/>
       <c r="P13" s="17"/>
     </row>
     <row r="14" spans="1:16" ht="118.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="17"/>
       <c r="B14" s="18"/>
-      <c r="C14" s="158"/>
-      <c r="D14" s="167" t="s">
+      <c r="C14" s="136"/>
+      <c r="D14" s="145" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="167"/>
-      <c r="F14" s="104" t="s">
+      <c r="E14" s="145"/>
+      <c r="F14" s="81" t="s">
         <v>26</v>
       </c>
       <c r="G14" s="51" t="s">
@@ -2925,7 +2607,7 @@
         <v>30</v>
       </c>
       <c r="K14" s="55" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="L14" s="42">
         <v>10</v>
@@ -2943,34 +2625,34 @@
     <row r="15" spans="1:16" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
       <c r="B15" s="27"/>
-      <c r="C15" s="119"/>
-      <c r="D15" s="168" t="s">
+      <c r="C15" s="95"/>
+      <c r="D15" s="146" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="161"/>
-      <c r="F15" s="161"/>
-      <c r="G15" s="161"/>
-      <c r="H15" s="161"/>
-      <c r="I15" s="161"/>
-      <c r="J15" s="161"/>
-      <c r="K15" s="161"/>
-      <c r="L15" s="106"/>
-      <c r="M15" s="106"/>
-      <c r="N15" s="106"/>
+      <c r="E15" s="139"/>
+      <c r="F15" s="139"/>
+      <c r="G15" s="139"/>
+      <c r="H15" s="139"/>
+      <c r="I15" s="139"/>
+      <c r="J15" s="139"/>
+      <c r="K15" s="139"/>
+      <c r="L15" s="83"/>
+      <c r="M15" s="83"/>
+      <c r="N15" s="83"/>
       <c r="O15" s="28"/>
       <c r="P15" s="17"/>
     </row>
     <row r="16" spans="1:16" ht="111.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="17"/>
       <c r="B16" s="18"/>
-      <c r="C16" s="119" t="s">
+      <c r="C16" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="141" t="s">
+      <c r="D16" s="119" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="162"/>
-      <c r="F16" s="104" t="s">
+      <c r="E16" s="140"/>
+      <c r="F16" s="81" t="s">
         <v>26</v>
       </c>
       <c r="G16" s="51" t="s">
@@ -2986,7 +2668,7 @@
         <v>37</v>
       </c>
       <c r="K16" s="55" t="s">
-        <v>38</v>
+        <v>198</v>
       </c>
       <c r="L16" s="42">
         <v>10</v>
@@ -3004,22 +2686,22 @@
     <row r="17" spans="1:23" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="17"/>
       <c r="B17" s="27"/>
-      <c r="C17" s="160" t="s">
+      <c r="C17" s="138" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="139" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="161" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="161"/>
-      <c r="F17" s="161"/>
-      <c r="G17" s="161"/>
-      <c r="H17" s="161"/>
-      <c r="I17" s="161"/>
-      <c r="J17" s="161"/>
-      <c r="K17" s="161"/>
-      <c r="L17" s="106"/>
-      <c r="M17" s="106"/>
-      <c r="N17" s="106"/>
+      <c r="E17" s="139"/>
+      <c r="F17" s="139"/>
+      <c r="G17" s="139"/>
+      <c r="H17" s="139"/>
+      <c r="I17" s="139"/>
+      <c r="J17" s="139"/>
+      <c r="K17" s="139"/>
+      <c r="L17" s="83"/>
+      <c r="M17" s="83"/>
+      <c r="N17" s="83"/>
       <c r="O17" s="28"/>
       <c r="P17" s="17"/>
       <c r="Q17" s="59"/>
@@ -3033,28 +2715,28 @@
     <row r="18" spans="1:23" ht="111.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="17"/>
       <c r="B18" s="18"/>
-      <c r="C18" s="160"/>
-      <c r="D18" s="141" t="s">
+      <c r="C18" s="138"/>
+      <c r="D18" s="119" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="140"/>
+      <c r="F18" s="81" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="162"/>
-      <c r="F18" s="104" t="s">
-        <v>26</v>
-      </c>
-      <c r="G18" s="51" t="s">
+      <c r="H18" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="H18" s="52" t="s">
+      <c r="I18" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="I18" s="53" t="s">
+      <c r="J18" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="J18" s="54" t="s">
+      <c r="K18" s="55" t="s">
         <v>45</v>
-      </c>
-      <c r="K18" s="55" t="s">
-        <v>46</v>
       </c>
       <c r="L18" s="42">
         <v>10</v>
@@ -3079,19 +2761,19 @@
     <row r="19" spans="1:23" ht="42.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="17"/>
       <c r="B19" s="27"/>
-      <c r="C19" s="158">
+      <c r="C19" s="136">
         <v>3</v>
       </c>
-      <c r="D19" s="163" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" s="164"/>
-      <c r="F19" s="164"/>
-      <c r="G19" s="164"/>
-      <c r="H19" s="164"/>
-      <c r="I19" s="164"/>
-      <c r="J19" s="164"/>
-      <c r="K19" s="164"/>
+      <c r="D19" s="141" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="142"/>
+      <c r="F19" s="142"/>
+      <c r="G19" s="142"/>
+      <c r="H19" s="142"/>
+      <c r="I19" s="142"/>
+      <c r="J19" s="142"/>
+      <c r="K19" s="142"/>
       <c r="L19" s="46"/>
       <c r="M19" s="46"/>
       <c r="N19" s="46"/>
@@ -3108,28 +2790,28 @@
     <row r="20" spans="1:23" s="57" customFormat="1" ht="111.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="49"/>
       <c r="B20" s="50"/>
-      <c r="C20" s="125"/>
-      <c r="D20" s="165" t="s">
+      <c r="C20" s="103"/>
+      <c r="D20" s="143" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="143"/>
+      <c r="F20" s="81" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="165"/>
-      <c r="F20" s="104" t="s">
-        <v>26</v>
-      </c>
-      <c r="G20" s="60" t="s">
+      <c r="H20" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="H20" s="61" t="s">
+      <c r="I20" s="62" t="s">
+        <v>199</v>
+      </c>
+      <c r="J20" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="I20" s="62" t="s">
-        <v>51</v>
-      </c>
-      <c r="J20" s="63" t="s">
-        <v>52</v>
-      </c>
       <c r="K20" s="64" t="s">
-        <v>53</v>
+        <v>200</v>
       </c>
       <c r="L20" s="42">
         <v>15</v>
@@ -3143,33 +2825,33 @@
       </c>
       <c r="O20" s="56"/>
       <c r="P20" s="49"/>
-      <c r="Q20" s="118"/>
-      <c r="R20" s="118"/>
-      <c r="S20" s="118"/>
-      <c r="T20" s="118"/>
-      <c r="U20" s="118"/>
-      <c r="V20" s="118"/>
-      <c r="W20" s="118"/>
+      <c r="Q20" s="94"/>
+      <c r="R20" s="94"/>
+      <c r="S20" s="94"/>
+      <c r="T20" s="94"/>
+      <c r="U20" s="94"/>
+      <c r="V20" s="94"/>
+      <c r="W20" s="94"/>
     </row>
     <row r="21" spans="1:23" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="17"/>
       <c r="B21" s="18"/>
-      <c r="C21" s="158" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="159" t="s">
-        <v>55</v>
-      </c>
-      <c r="E21" s="140"/>
-      <c r="F21" s="140"/>
-      <c r="G21" s="140"/>
-      <c r="H21" s="140"/>
-      <c r="I21" s="140"/>
-      <c r="J21" s="109"/>
-      <c r="K21" s="109"/>
-      <c r="L21" s="106"/>
-      <c r="M21" s="106"/>
-      <c r="N21" s="106"/>
+      <c r="C21" s="136" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="137" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="118"/>
+      <c r="F21" s="118"/>
+      <c r="G21" s="118"/>
+      <c r="H21" s="118"/>
+      <c r="I21" s="118"/>
+      <c r="J21" s="86"/>
+      <c r="K21" s="86"/>
+      <c r="L21" s="83"/>
+      <c r="M21" s="83"/>
+      <c r="N21" s="83"/>
       <c r="O21" s="28"/>
       <c r="P21" s="17"/>
       <c r="Q21" s="59"/>
@@ -3183,28 +2865,28 @@
     <row r="22" spans="1:23" ht="138.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17"/>
       <c r="B22" s="18"/>
-      <c r="C22" s="125"/>
-      <c r="D22" s="141" t="s">
+      <c r="C22" s="103"/>
+      <c r="D22" s="119" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="119"/>
+      <c r="F22" s="81" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="H22" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="I22" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="E22" s="141"/>
-      <c r="F22" s="104" t="s">
-        <v>26</v>
-      </c>
-      <c r="G22" s="58" t="s">
+      <c r="J22" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="H22" s="41" t="s">
+      <c r="K22" s="48" t="s">
         <v>58</v>
-      </c>
-      <c r="I22" s="47" t="s">
-        <v>59</v>
-      </c>
-      <c r="J22" s="63" t="s">
-        <v>60</v>
-      </c>
-      <c r="K22" s="48" t="s">
-        <v>61</v>
       </c>
       <c r="L22" s="42">
         <v>15</v>
@@ -3230,19 +2912,19 @@
       <c r="A23" s="17"/>
       <c r="B23" s="18"/>
       <c r="C23" s="59"/>
-      <c r="D23" s="140" t="s">
-        <v>62</v>
-      </c>
-      <c r="E23" s="140"/>
-      <c r="F23" s="140"/>
-      <c r="G23" s="140"/>
-      <c r="H23" s="140"/>
-      <c r="I23" s="140"/>
-      <c r="J23" s="109"/>
-      <c r="K23" s="109"/>
-      <c r="L23" s="106"/>
-      <c r="M23" s="106"/>
-      <c r="N23" s="106"/>
+      <c r="D23" s="118" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" s="118"/>
+      <c r="F23" s="118"/>
+      <c r="G23" s="118"/>
+      <c r="H23" s="118"/>
+      <c r="I23" s="118"/>
+      <c r="J23" s="86"/>
+      <c r="K23" s="86"/>
+      <c r="L23" s="83"/>
+      <c r="M23" s="83"/>
+      <c r="N23" s="83"/>
       <c r="O23" s="28"/>
       <c r="P23" s="17"/>
       <c r="Q23" s="59"/>
@@ -3257,29 +2939,29 @@
       <c r="A24" s="17"/>
       <c r="B24" s="18"/>
       <c r="C24" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="119" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24" s="119"/>
+      <c r="F24" s="81" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="58" t="s">
+        <v>62</v>
+      </c>
+      <c r="H24" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="141" t="s">
+      <c r="I24" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="E24" s="141"/>
-      <c r="F24" s="104" t="s">
-        <v>26</v>
-      </c>
-      <c r="G24" s="58" t="s">
+      <c r="J24" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="H24" s="41" t="s">
+      <c r="K24" s="48" t="s">
         <v>66</v>
-      </c>
-      <c r="I24" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="J24" s="63" t="s">
-        <v>68</v>
-      </c>
-      <c r="K24" s="48" t="s">
-        <v>69</v>
       </c>
       <c r="L24" s="42">
         <v>20</v>
@@ -3305,19 +2987,19 @@
       <c r="A25" s="17"/>
       <c r="B25" s="18"/>
       <c r="C25" s="59"/>
-      <c r="D25" s="140" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="140"/>
-      <c r="F25" s="140"/>
-      <c r="G25" s="140"/>
-      <c r="H25" s="140"/>
-      <c r="I25" s="140"/>
-      <c r="J25" s="109"/>
-      <c r="K25" s="109"/>
-      <c r="L25" s="106"/>
-      <c r="M25" s="106"/>
-      <c r="N25" s="106"/>
+      <c r="D25" s="118" t="s">
+        <v>206</v>
+      </c>
+      <c r="E25" s="118"/>
+      <c r="F25" s="118"/>
+      <c r="G25" s="118"/>
+      <c r="H25" s="118"/>
+      <c r="I25" s="118"/>
+      <c r="J25" s="86"/>
+      <c r="K25" s="86"/>
+      <c r="L25" s="83"/>
+      <c r="M25" s="83"/>
+      <c r="N25" s="83"/>
       <c r="O25" s="28"/>
       <c r="P25" s="17"/>
       <c r="Q25" s="59"/>
@@ -3332,29 +3014,29 @@
       <c r="A26" s="17"/>
       <c r="B26" s="18"/>
       <c r="C26" s="59" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" s="141" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="119" t="s">
+        <v>207</v>
+      </c>
+      <c r="E26" s="119"/>
+      <c r="F26" s="81" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="H26" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="I26" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="J26" s="63" t="s">
+        <v>70</v>
+      </c>
+      <c r="K26" s="48" t="s">
         <v>71</v>
-      </c>
-      <c r="E26" s="141"/>
-      <c r="F26" s="104" t="s">
-        <v>26</v>
-      </c>
-      <c r="G26" s="58" t="s">
-        <v>72</v>
-      </c>
-      <c r="H26" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="I26" s="47" t="s">
-        <v>74</v>
-      </c>
-      <c r="J26" s="63" t="s">
-        <v>75</v>
-      </c>
-      <c r="K26" s="48" t="s">
-        <v>76</v>
       </c>
       <c r="L26" s="42">
         <v>20</v>
@@ -3387,10 +3069,20 @@
       <c r="H27" s="18"/>
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="18"/>
+      <c r="K27" s="97" t="s">
+        <v>196</v>
+      </c>
+      <c r="L27" s="97">
+        <f>SUM(L14,L16,L18,L20,L22,L24,L26)</f>
+        <v>100</v>
+      </c>
+      <c r="M27" s="98" t="s">
+        <v>197</v>
+      </c>
+      <c r="N27" s="98">
+        <f>SUM(N14,N16,N18,N20,N22,N24,N26)</f>
+        <v>0</v>
+      </c>
       <c r="O27" s="28"/>
       <c r="P27" s="17"/>
       <c r="Q27" s="59"/>
@@ -3422,11 +3114,11 @@
     <row r="29" spans="1:23" s="59" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A29" s="17"/>
       <c r="B29" s="29"/>
-      <c r="C29" s="124" t="s">
-        <v>77</v>
-      </c>
-      <c r="D29" s="125"/>
-      <c r="E29" s="125"/>
+      <c r="C29" s="102" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="103"/>
+      <c r="E29" s="103"/>
       <c r="F29" s="29"/>
       <c r="G29" s="29"/>
       <c r="H29" s="29"/>
@@ -3442,27 +3134,27 @@
     <row r="30" spans="1:23" s="59" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
       <c r="B30" s="29"/>
-      <c r="C30" s="112" t="s">
-        <v>78</v>
-      </c>
-      <c r="D30" s="127" t="s">
-        <v>79</v>
-      </c>
-      <c r="E30" s="125"/>
-      <c r="F30" s="112" t="s">
-        <v>80</v>
-      </c>
-      <c r="G30" s="127" t="s">
+      <c r="C30" s="89" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="105" t="s">
+        <v>74</v>
+      </c>
+      <c r="E30" s="103"/>
+      <c r="F30" s="89" t="s">
+        <v>75</v>
+      </c>
+      <c r="G30" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="H30" s="125"/>
-      <c r="I30" s="125"/>
-      <c r="J30" s="125"/>
-      <c r="K30" s="125"/>
+      <c r="H30" s="103"/>
+      <c r="I30" s="103"/>
+      <c r="J30" s="103"/>
+      <c r="K30" s="103"/>
       <c r="L30" s="65"/>
-      <c r="M30" s="112"/>
-      <c r="N30" s="115" t="s">
-        <v>81</v>
+      <c r="M30" s="89"/>
+      <c r="N30" s="92" t="s">
+        <v>76</v>
       </c>
       <c r="O30" s="29"/>
       <c r="P30" s="17"/>
@@ -3473,22 +3165,22 @@
       <c r="C31" s="66">
         <v>9</v>
       </c>
-      <c r="D31" s="137" t="s">
-        <v>82</v>
-      </c>
-      <c r="E31" s="138"/>
-      <c r="F31" s="114" t="s">
-        <v>83</v>
-      </c>
-      <c r="G31" s="139" t="s">
-        <v>84</v>
-      </c>
-      <c r="H31" s="139"/>
-      <c r="I31" s="139"/>
-      <c r="J31" s="139"/>
-      <c r="K31" s="139"/>
-      <c r="L31" s="139"/>
-      <c r="M31" s="139"/>
+      <c r="D31" s="115" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" s="116"/>
+      <c r="F31" s="91" t="s">
+        <v>78</v>
+      </c>
+      <c r="G31" s="117" t="s">
+        <v>79</v>
+      </c>
+      <c r="H31" s="117"/>
+      <c r="I31" s="117"/>
+      <c r="J31" s="117"/>
+      <c r="K31" s="117"/>
+      <c r="L31" s="117"/>
+      <c r="M31" s="117"/>
       <c r="N31" s="67">
         <v>3</v>
       </c>
@@ -3501,22 +3193,22 @@
       <c r="C32" s="68">
         <v>10</v>
       </c>
-      <c r="D32" s="142" t="s">
-        <v>82</v>
-      </c>
-      <c r="E32" s="138"/>
-      <c r="F32" s="114" t="s">
-        <v>85</v>
-      </c>
-      <c r="G32" s="139" t="s">
-        <v>86</v>
-      </c>
-      <c r="H32" s="139"/>
-      <c r="I32" s="139"/>
-      <c r="J32" s="139"/>
-      <c r="K32" s="139"/>
-      <c r="L32" s="139"/>
-      <c r="M32" s="139"/>
+      <c r="D32" s="120" t="s">
+        <v>77</v>
+      </c>
+      <c r="E32" s="116"/>
+      <c r="F32" s="91" t="s">
+        <v>80</v>
+      </c>
+      <c r="G32" s="117" t="s">
+        <v>81</v>
+      </c>
+      <c r="H32" s="117"/>
+      <c r="I32" s="117"/>
+      <c r="J32" s="117"/>
+      <c r="K32" s="117"/>
+      <c r="L32" s="117"/>
+      <c r="M32" s="117"/>
       <c r="N32" s="69">
         <v>3</v>
       </c>
@@ -3529,22 +3221,22 @@
       <c r="C33" s="66">
         <v>11</v>
       </c>
-      <c r="D33" s="137" t="s">
+      <c r="D33" s="115" t="s">
+        <v>77</v>
+      </c>
+      <c r="E33" s="116"/>
+      <c r="F33" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="E33" s="138"/>
-      <c r="F33" s="114" t="s">
-        <v>87</v>
-      </c>
-      <c r="G33" s="139" t="s">
-        <v>88</v>
-      </c>
-      <c r="H33" s="139"/>
-      <c r="I33" s="139"/>
-      <c r="J33" s="139"/>
-      <c r="K33" s="139"/>
-      <c r="L33" s="139"/>
-      <c r="M33" s="139"/>
+      <c r="G33" s="117" t="s">
+        <v>83</v>
+      </c>
+      <c r="H33" s="117"/>
+      <c r="I33" s="117"/>
+      <c r="J33" s="117"/>
+      <c r="K33" s="117"/>
+      <c r="L33" s="117"/>
+      <c r="M33" s="117"/>
       <c r="N33" s="67">
         <v>3</v>
       </c>
@@ -3557,22 +3249,22 @@
       <c r="C34" s="70">
         <v>1</v>
       </c>
-      <c r="D34" s="135" t="s">
-        <v>89</v>
-      </c>
-      <c r="E34" s="135"/>
-      <c r="F34" s="113" t="s">
-        <v>90</v>
-      </c>
-      <c r="G34" s="133" t="s">
-        <v>91</v>
-      </c>
-      <c r="H34" s="133"/>
-      <c r="I34" s="133"/>
-      <c r="J34" s="133"/>
-      <c r="K34" s="133"/>
-      <c r="L34" s="133"/>
-      <c r="M34" s="133"/>
+      <c r="D34" s="113" t="s">
+        <v>84</v>
+      </c>
+      <c r="E34" s="113"/>
+      <c r="F34" s="90" t="s">
+        <v>85</v>
+      </c>
+      <c r="G34" s="111" t="s">
+        <v>205</v>
+      </c>
+      <c r="H34" s="111"/>
+      <c r="I34" s="111"/>
+      <c r="J34" s="111"/>
+      <c r="K34" s="111"/>
+      <c r="L34" s="111"/>
+      <c r="M34" s="111"/>
       <c r="N34" s="71">
         <v>3</v>
       </c>
@@ -3585,22 +3277,22 @@
       <c r="C35" s="72">
         <v>2</v>
       </c>
-      <c r="D35" s="128" t="s">
-        <v>89</v>
-      </c>
-      <c r="E35" s="129"/>
-      <c r="F35" s="110" t="s">
-        <v>92</v>
-      </c>
-      <c r="G35" s="130" t="s">
-        <v>93</v>
-      </c>
-      <c r="H35" s="130"/>
-      <c r="I35" s="130"/>
-      <c r="J35" s="130"/>
-      <c r="K35" s="130"/>
-      <c r="L35" s="130"/>
-      <c r="M35" s="130"/>
+      <c r="D35" s="106" t="s">
+        <v>84</v>
+      </c>
+      <c r="E35" s="107"/>
+      <c r="F35" s="87" t="s">
+        <v>86</v>
+      </c>
+      <c r="G35" s="108" t="s">
+        <v>87</v>
+      </c>
+      <c r="H35" s="108"/>
+      <c r="I35" s="108"/>
+      <c r="J35" s="108"/>
+      <c r="K35" s="108"/>
+      <c r="L35" s="108"/>
+      <c r="M35" s="108"/>
       <c r="N35" s="73">
         <v>3</v>
       </c>
@@ -3613,22 +3305,22 @@
       <c r="C36" s="74">
         <v>3</v>
       </c>
-      <c r="D36" s="131" t="s">
-        <v>94</v>
-      </c>
-      <c r="E36" s="132"/>
-      <c r="F36" s="113" t="s">
-        <v>95</v>
-      </c>
-      <c r="G36" s="133" t="s">
-        <v>96</v>
-      </c>
-      <c r="H36" s="133"/>
-      <c r="I36" s="133"/>
-      <c r="J36" s="133"/>
-      <c r="K36" s="133"/>
-      <c r="L36" s="133"/>
-      <c r="M36" s="133"/>
+      <c r="D36" s="109" t="s">
+        <v>88</v>
+      </c>
+      <c r="E36" s="110"/>
+      <c r="F36" s="90" t="s">
+        <v>89</v>
+      </c>
+      <c r="G36" s="111" t="s">
+        <v>90</v>
+      </c>
+      <c r="H36" s="111"/>
+      <c r="I36" s="111"/>
+      <c r="J36" s="111"/>
+      <c r="K36" s="111"/>
+      <c r="L36" s="111"/>
+      <c r="M36" s="111"/>
       <c r="N36" s="75">
         <v>3</v>
       </c>
@@ -3641,22 +3333,22 @@
       <c r="C37" s="76">
         <v>4</v>
       </c>
-      <c r="D37" s="134" t="s">
-        <v>97</v>
-      </c>
-      <c r="E37" s="129"/>
-      <c r="F37" s="110" t="s">
-        <v>98</v>
-      </c>
-      <c r="G37" s="130" t="s">
-        <v>99</v>
-      </c>
-      <c r="H37" s="130"/>
-      <c r="I37" s="130"/>
-      <c r="J37" s="130"/>
-      <c r="K37" s="130"/>
-      <c r="L37" s="130"/>
-      <c r="M37" s="130"/>
+      <c r="D37" s="112" t="s">
+        <v>91</v>
+      </c>
+      <c r="E37" s="107"/>
+      <c r="F37" s="87" t="s">
+        <v>92</v>
+      </c>
+      <c r="G37" s="108" t="s">
+        <v>202</v>
+      </c>
+      <c r="H37" s="108"/>
+      <c r="I37" s="108"/>
+      <c r="J37" s="108"/>
+      <c r="K37" s="108"/>
+      <c r="L37" s="108"/>
+      <c r="M37" s="108"/>
       <c r="N37" s="77">
         <v>3</v>
       </c>
@@ -3669,22 +3361,22 @@
       <c r="C38" s="70">
         <v>5</v>
       </c>
-      <c r="D38" s="135" t="s">
-        <v>100</v>
-      </c>
-      <c r="E38" s="136"/>
-      <c r="F38" s="113" t="s">
-        <v>100</v>
-      </c>
-      <c r="G38" s="133" t="s">
-        <v>101</v>
-      </c>
-      <c r="H38" s="133"/>
-      <c r="I38" s="133"/>
-      <c r="J38" s="133"/>
-      <c r="K38" s="133"/>
-      <c r="L38" s="133"/>
-      <c r="M38" s="133"/>
+      <c r="D38" s="113" t="s">
+        <v>93</v>
+      </c>
+      <c r="E38" s="114"/>
+      <c r="F38" s="90" t="s">
+        <v>93</v>
+      </c>
+      <c r="G38" s="111" t="s">
+        <v>203</v>
+      </c>
+      <c r="H38" s="111"/>
+      <c r="I38" s="111"/>
+      <c r="J38" s="111"/>
+      <c r="K38" s="111"/>
+      <c r="L38" s="111"/>
+      <c r="M38" s="111"/>
       <c r="N38" s="71">
         <v>3</v>
       </c>
@@ -3697,22 +3389,22 @@
       <c r="C39" s="72">
         <v>6</v>
       </c>
-      <c r="D39" s="128" t="s">
-        <v>100</v>
-      </c>
-      <c r="E39" s="129"/>
-      <c r="F39" s="110" t="s">
-        <v>102</v>
-      </c>
-      <c r="G39" s="130" t="s">
-        <v>103</v>
-      </c>
-      <c r="H39" s="130"/>
-      <c r="I39" s="130"/>
-      <c r="J39" s="130"/>
-      <c r="K39" s="130"/>
-      <c r="L39" s="130"/>
-      <c r="M39" s="130"/>
+      <c r="D39" s="106" t="s">
+        <v>93</v>
+      </c>
+      <c r="E39" s="107"/>
+      <c r="F39" s="87" t="s">
+        <v>94</v>
+      </c>
+      <c r="G39" s="108" t="s">
+        <v>204</v>
+      </c>
+      <c r="H39" s="108"/>
+      <c r="I39" s="108"/>
+      <c r="J39" s="108"/>
+      <c r="K39" s="108"/>
+      <c r="L39" s="108"/>
+      <c r="M39" s="108"/>
       <c r="N39" s="73">
         <v>3</v>
       </c>
@@ -3725,22 +3417,22 @@
       <c r="C40" s="74">
         <v>7</v>
       </c>
-      <c r="D40" s="131" t="s">
-        <v>104</v>
-      </c>
-      <c r="E40" s="132"/>
-      <c r="F40" s="113" t="s">
-        <v>105</v>
-      </c>
-      <c r="G40" s="133" t="s">
-        <v>106</v>
-      </c>
-      <c r="H40" s="133"/>
-      <c r="I40" s="133"/>
-      <c r="J40" s="133"/>
-      <c r="K40" s="133"/>
-      <c r="L40" s="133"/>
-      <c r="M40" s="133"/>
+      <c r="D40" s="109" t="s">
+        <v>95</v>
+      </c>
+      <c r="E40" s="110"/>
+      <c r="F40" s="90" t="s">
+        <v>96</v>
+      </c>
+      <c r="G40" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="H40" s="111"/>
+      <c r="I40" s="111"/>
+      <c r="J40" s="111"/>
+      <c r="K40" s="111"/>
+      <c r="L40" s="111"/>
+      <c r="M40" s="111"/>
       <c r="N40" s="75">
         <v>3</v>
       </c>
@@ -3753,22 +3445,22 @@
       <c r="C41" s="76">
         <v>8</v>
       </c>
-      <c r="D41" s="134" t="s">
-        <v>104</v>
-      </c>
-      <c r="E41" s="129"/>
-      <c r="F41" s="110" t="s">
-        <v>107</v>
-      </c>
-      <c r="G41" s="130" t="s">
-        <v>108</v>
-      </c>
-      <c r="H41" s="130"/>
-      <c r="I41" s="130"/>
-      <c r="J41" s="130"/>
-      <c r="K41" s="130"/>
-      <c r="L41" s="130"/>
-      <c r="M41" s="130"/>
+      <c r="D41" s="112" t="s">
+        <v>95</v>
+      </c>
+      <c r="E41" s="107"/>
+      <c r="F41" s="87" t="s">
+        <v>98</v>
+      </c>
+      <c r="G41" s="108" t="s">
+        <v>99</v>
+      </c>
+      <c r="H41" s="108"/>
+      <c r="I41" s="108"/>
+      <c r="J41" s="108"/>
+      <c r="K41" s="108"/>
+      <c r="L41" s="108"/>
+      <c r="M41" s="108"/>
       <c r="N41" s="77">
         <v>3</v>
       </c>
@@ -3814,11 +3506,11 @@
     <row r="44" spans="1:16" s="59" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A44" s="17"/>
       <c r="B44" s="32"/>
-      <c r="C44" s="124" t="s">
-        <v>109</v>
-      </c>
-      <c r="D44" s="125"/>
-      <c r="E44" s="125"/>
+      <c r="C44" s="102" t="s">
+        <v>100</v>
+      </c>
+      <c r="D44" s="103"/>
+      <c r="E44" s="103"/>
       <c r="F44" s="27"/>
       <c r="G44" s="18"/>
       <c r="H44" s="18"/>
@@ -3835,25 +3527,25 @@
       <c r="A45" s="17"/>
       <c r="B45" s="32"/>
       <c r="C45" s="33" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D45" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="E45" s="111"/>
-      <c r="F45" s="126" t="s">
-        <v>111</v>
-      </c>
-      <c r="G45" s="125"/>
-      <c r="H45" s="125"/>
-      <c r="I45" s="125"/>
-      <c r="J45" s="127" t="s">
-        <v>112</v>
-      </c>
-      <c r="K45" s="125"/>
-      <c r="L45" s="125"/>
-      <c r="M45" s="125"/>
-      <c r="N45" s="125"/>
+        <v>101</v>
+      </c>
+      <c r="E45" s="88"/>
+      <c r="F45" s="104" t="s">
+        <v>102</v>
+      </c>
+      <c r="G45" s="103"/>
+      <c r="H45" s="103"/>
+      <c r="I45" s="103"/>
+      <c r="J45" s="105" t="s">
+        <v>103</v>
+      </c>
+      <c r="K45" s="103"/>
+      <c r="L45" s="103"/>
+      <c r="M45" s="103"/>
+      <c r="N45" s="103"/>
       <c r="O45" s="18"/>
       <c r="P45" s="17"/>
     </row>
@@ -3864,22 +3556,22 @@
         <v>1</v>
       </c>
       <c r="D46" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="E46" s="108"/>
-      <c r="F46" s="121" t="s">
-        <v>114</v>
-      </c>
-      <c r="G46" s="122"/>
-      <c r="H46" s="122"/>
-      <c r="I46" s="122"/>
-      <c r="J46" s="121" t="s">
-        <v>115</v>
-      </c>
-      <c r="K46" s="122"/>
-      <c r="L46" s="122"/>
-      <c r="M46" s="122"/>
-      <c r="N46" s="122"/>
+        <v>104</v>
+      </c>
+      <c r="E46" s="85"/>
+      <c r="F46" s="99" t="s">
+        <v>105</v>
+      </c>
+      <c r="G46" s="100"/>
+      <c r="H46" s="100"/>
+      <c r="I46" s="100"/>
+      <c r="J46" s="99" t="s">
+        <v>106</v>
+      </c>
+      <c r="K46" s="100"/>
+      <c r="L46" s="100"/>
+      <c r="M46" s="100"/>
+      <c r="N46" s="100"/>
       <c r="O46" s="18"/>
       <c r="P46" s="17"/>
     </row>
@@ -3890,22 +3582,22 @@
         <v>2</v>
       </c>
       <c r="D47" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="E47" s="107"/>
-      <c r="F47" s="123" t="s">
-        <v>117</v>
-      </c>
-      <c r="G47" s="122"/>
-      <c r="H47" s="122"/>
-      <c r="I47" s="122"/>
-      <c r="J47" s="123" t="s">
-        <v>118</v>
-      </c>
-      <c r="K47" s="122"/>
-      <c r="L47" s="122"/>
-      <c r="M47" s="122"/>
-      <c r="N47" s="122"/>
+        <v>107</v>
+      </c>
+      <c r="E47" s="84"/>
+      <c r="F47" s="101" t="s">
+        <v>108</v>
+      </c>
+      <c r="G47" s="100"/>
+      <c r="H47" s="100"/>
+      <c r="I47" s="100"/>
+      <c r="J47" s="101" t="s">
+        <v>109</v>
+      </c>
+      <c r="K47" s="100"/>
+      <c r="L47" s="100"/>
+      <c r="M47" s="100"/>
+      <c r="N47" s="100"/>
       <c r="O47" s="18"/>
       <c r="P47" s="17"/>
     </row>
@@ -3916,22 +3608,22 @@
         <v>3</v>
       </c>
       <c r="D48" s="36" t="s">
-        <v>119</v>
-      </c>
-      <c r="E48" s="108"/>
-      <c r="F48" s="121" t="s">
-        <v>120</v>
-      </c>
-      <c r="G48" s="122"/>
-      <c r="H48" s="122"/>
-      <c r="I48" s="122"/>
-      <c r="J48" s="121" t="s">
-        <v>121</v>
-      </c>
-      <c r="K48" s="122"/>
-      <c r="L48" s="122"/>
-      <c r="M48" s="122"/>
-      <c r="N48" s="122"/>
+        <v>110</v>
+      </c>
+      <c r="E48" s="85"/>
+      <c r="F48" s="99" t="s">
+        <v>111</v>
+      </c>
+      <c r="G48" s="100"/>
+      <c r="H48" s="100"/>
+      <c r="I48" s="100"/>
+      <c r="J48" s="99" t="s">
+        <v>112</v>
+      </c>
+      <c r="K48" s="100"/>
+      <c r="L48" s="100"/>
+      <c r="M48" s="100"/>
+      <c r="N48" s="100"/>
       <c r="O48" s="18"/>
       <c r="P48" s="17"/>
     </row>
@@ -3942,22 +3634,22 @@
         <v>4</v>
       </c>
       <c r="D49" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="E49" s="107"/>
-      <c r="F49" s="123" t="s">
-        <v>123</v>
-      </c>
-      <c r="G49" s="122"/>
-      <c r="H49" s="122"/>
-      <c r="I49" s="122"/>
-      <c r="J49" s="123" t="s">
-        <v>124</v>
-      </c>
-      <c r="K49" s="122"/>
-      <c r="L49" s="122"/>
-      <c r="M49" s="122"/>
-      <c r="N49" s="122"/>
+        <v>113</v>
+      </c>
+      <c r="E49" s="84"/>
+      <c r="F49" s="101" t="s">
+        <v>114</v>
+      </c>
+      <c r="G49" s="100"/>
+      <c r="H49" s="100"/>
+      <c r="I49" s="100"/>
+      <c r="J49" s="101" t="s">
+        <v>115</v>
+      </c>
+      <c r="K49" s="100"/>
+      <c r="L49" s="100"/>
+      <c r="M49" s="100"/>
+      <c r="N49" s="100"/>
       <c r="O49" s="18"/>
       <c r="P49" s="17"/>
     </row>
@@ -3968,22 +3660,22 @@
         <v>5</v>
       </c>
       <c r="D50" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="E50" s="108"/>
-      <c r="F50" s="121" t="s">
-        <v>126</v>
-      </c>
-      <c r="G50" s="122"/>
-      <c r="H50" s="122"/>
-      <c r="I50" s="122"/>
-      <c r="J50" s="121" t="s">
-        <v>127</v>
-      </c>
-      <c r="K50" s="122"/>
-      <c r="L50" s="122"/>
-      <c r="M50" s="122"/>
-      <c r="N50" s="122"/>
+        <v>116</v>
+      </c>
+      <c r="E50" s="85"/>
+      <c r="F50" s="99" t="s">
+        <v>117</v>
+      </c>
+      <c r="G50" s="100"/>
+      <c r="H50" s="100"/>
+      <c r="I50" s="100"/>
+      <c r="J50" s="99" t="s">
+        <v>118</v>
+      </c>
+      <c r="K50" s="100"/>
+      <c r="L50" s="100"/>
+      <c r="M50" s="100"/>
+      <c r="N50" s="100"/>
       <c r="O50" s="18"/>
       <c r="P50" s="17"/>
     </row>
@@ -4282,7 +3974,7 @@
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4299,219 +3991,119 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="176" t="s">
-        <v>128</v>
-      </c>
-      <c r="B1" s="177"/>
-      <c r="C1" s="177"/>
-      <c r="D1" s="177"/>
-      <c r="E1" s="177"/>
-      <c r="F1" s="177"/>
-      <c r="G1" s="177"/>
-      <c r="H1" s="178"/>
+      <c r="A1" s="149"/>
+      <c r="B1" s="149"/>
+      <c r="C1" s="149"/>
+      <c r="D1" s="149"/>
+      <c r="E1" s="149"/>
+      <c r="F1" s="149"/>
+      <c r="G1" s="149"/>
+      <c r="H1" s="149"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="179"/>
-      <c r="B2" s="180"/>
-      <c r="C2" s="180"/>
-      <c r="D2" s="180"/>
-      <c r="E2" s="180"/>
-      <c r="F2" s="180"/>
-      <c r="G2" s="180"/>
-      <c r="H2" s="181"/>
+      <c r="A2" s="149"/>
+      <c r="B2" s="149"/>
+      <c r="C2" s="149"/>
+      <c r="D2" s="149"/>
+      <c r="E2" s="149"/>
+      <c r="F2" s="149"/>
+      <c r="G2" s="149"/>
+      <c r="H2" s="149"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="174" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="175"/>
-      <c r="C3" s="116" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="171" t="s">
-        <v>109</v>
-      </c>
-      <c r="E3" s="172"/>
-      <c r="F3" s="172"/>
-      <c r="G3" s="172"/>
-      <c r="H3" s="173"/>
-      <c r="K3" s="169"/>
-      <c r="L3" s="170"/>
-      <c r="M3" s="170"/>
-      <c r="N3" s="170"/>
-      <c r="O3" s="100"/>
+      <c r="A3" s="149"/>
+      <c r="B3" s="149"/>
+      <c r="C3"/>
+      <c r="D3" s="149"/>
+      <c r="E3" s="149"/>
+      <c r="F3" s="149"/>
+      <c r="G3" s="149"/>
+      <c r="H3" s="149"/>
+      <c r="K3" s="147"/>
+      <c r="L3" s="148"/>
+      <c r="M3" s="148"/>
+      <c r="N3" s="148"/>
+      <c r="O3" s="80"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="99"/>
-      <c r="B4" s="98"/>
-      <c r="C4" s="98"/>
-      <c r="D4" s="97">
-        <v>1</v>
-      </c>
-      <c r="E4" s="96">
-        <v>2</v>
-      </c>
-      <c r="F4" s="96">
-        <v>3</v>
-      </c>
-      <c r="G4" s="96">
-        <v>4</v>
-      </c>
-      <c r="H4" s="95">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="91"/>
-      <c r="D5" s="94" t="s">
-        <v>129</v>
-      </c>
-      <c r="E5" s="93" t="s">
-        <v>130</v>
-      </c>
-      <c r="F5" s="93" t="s">
-        <v>119</v>
-      </c>
-      <c r="G5" s="93" t="s">
-        <v>122</v>
-      </c>
-      <c r="H5" s="92" t="s">
-        <v>125</v>
-      </c>
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="91"/>
-      <c r="D6" s="90"/>
-      <c r="E6" s="89"/>
-      <c r="F6" s="89"/>
-      <c r="G6" s="89"/>
-      <c r="H6" s="88"/>
-    </row>
-    <row r="7" spans="1:15" s="84" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="101">
-        <v>5</v>
-      </c>
-      <c r="B7" s="102" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" s="102" t="s">
-        <v>131</v>
-      </c>
-      <c r="D7" s="101" t="s">
-        <v>132</v>
-      </c>
-      <c r="E7" s="101" t="s">
-        <v>132</v>
-      </c>
-      <c r="F7" s="101" t="s">
-        <v>132</v>
-      </c>
-      <c r="G7" s="101"/>
-      <c r="H7" s="101" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" s="84" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="101">
-        <v>6</v>
-      </c>
-      <c r="B8" s="103" t="s">
-        <v>102</v>
-      </c>
-      <c r="C8" s="102" t="s">
-        <v>133</v>
-      </c>
-      <c r="D8" s="101" t="s">
-        <v>132</v>
-      </c>
-      <c r="E8" s="101" t="s">
-        <v>132</v>
-      </c>
-      <c r="F8" s="101" t="s">
-        <v>132</v>
-      </c>
-      <c r="G8" s="101" t="s">
-        <v>132</v>
-      </c>
-      <c r="H8" s="101" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" s="84" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="87">
-        <v>9</v>
-      </c>
-      <c r="B9" s="82" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="81" t="s">
-        <v>134</v>
-      </c>
-      <c r="D9" s="85" t="s">
-        <v>132</v>
-      </c>
-      <c r="E9" s="86" t="s">
-        <v>132</v>
-      </c>
-      <c r="F9" s="86" t="s">
-        <v>132</v>
-      </c>
-      <c r="G9" s="85" t="s">
-        <v>132</v>
-      </c>
-      <c r="H9" s="85"/>
-    </row>
-    <row r="10" spans="1:15" s="84" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="87">
-        <v>10</v>
-      </c>
-      <c r="B10" s="82" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" s="81" t="s">
-        <v>135</v>
-      </c>
-      <c r="D10" s="85" t="s">
-        <v>132</v>
-      </c>
-      <c r="E10" s="86" t="s">
-        <v>132</v>
-      </c>
-      <c r="F10" s="86" t="s">
-        <v>132</v>
-      </c>
-      <c r="G10" s="85" t="s">
-        <v>132</v>
-      </c>
-      <c r="H10" s="85" t="s">
-        <v>132</v>
-      </c>
+      <c r="A6"/>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+    </row>
+    <row r="7" spans="1:15" s="79" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7"/>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+    </row>
+    <row r="8" spans="1:15" s="79" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+    </row>
+    <row r="9" spans="1:15" s="79" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+    </row>
+    <row r="10" spans="1:15" s="79" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
     </row>
     <row r="11" spans="1:15" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="83">
-        <v>11</v>
-      </c>
-      <c r="B11" s="82" t="s">
-        <v>87</v>
-      </c>
-      <c r="C11" s="81" t="s">
-        <v>136</v>
-      </c>
-      <c r="D11" s="79" t="s">
-        <v>132</v>
-      </c>
-      <c r="E11" s="80" t="s">
-        <v>132</v>
-      </c>
-      <c r="F11" s="80" t="s">
-        <v>132</v>
-      </c>
-      <c r="G11" s="79" t="s">
-        <v>132</v>
-      </c>
-      <c r="H11" s="79" t="s">
-        <v>132</v>
-      </c>
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4541,37 +4133,37 @@
   <sheetData>
     <row r="2" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="B2" s="184" t="s">
-        <v>138</v>
-      </c>
-      <c r="C2" s="145"/>
-      <c r="D2" s="145"/>
+        <v>119</v>
+      </c>
+      <c r="B2" s="152" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
       <c r="G2" s="4"/>
       <c r="H2" s="1" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B3" s="117"/>
-      <c r="C3" s="117"/>
-      <c r="D3" s="117"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
       <c r="F3" s="10"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -4589,9 +4181,9 @@
       <c r="T3" s="4"/>
     </row>
     <row r="4" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B4" s="117"/>
-      <c r="C4" s="117"/>
-      <c r="D4" s="117"/>
+      <c r="B4" s="93"/>
+      <c r="C4" s="93"/>
+      <c r="D4" s="93"/>
       <c r="F4" s="10"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -4609,34 +4201,34 @@
       <c r="T4" s="4"/>
     </row>
     <row r="5" spans="1:20" ht="191.25" x14ac:dyDescent="0.2">
-      <c r="B5" s="182" t="s">
-        <v>145</v>
-      </c>
-      <c r="C5" s="145"/>
-      <c r="D5" s="145"/>
+      <c r="B5" s="150" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" s="123"/>
+      <c r="D5" s="123"/>
       <c r="F5" s="10">
         <v>6.1</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="N5" s="2" t="e">
         <f ca="1">_xludf.CONCAT(M5,M6)</f>
@@ -4665,27 +4257,27 @@
       <c r="T5" s="4"/>
     </row>
     <row r="6" spans="1:20" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="B6" s="117"/>
-      <c r="C6" s="117"/>
-      <c r="D6" s="117"/>
+      <c r="B6" s="93"/>
+      <c r="C6" s="93"/>
+      <c r="D6" s="93"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -4696,34 +4288,34 @@
       <c r="T6" s="4"/>
     </row>
     <row r="7" spans="1:20" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="B7" s="182" t="s">
-        <v>159</v>
-      </c>
-      <c r="C7" s="145"/>
-      <c r="D7" s="145"/>
+      <c r="B7" s="150" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" s="123"/>
+      <c r="D7" s="123"/>
       <c r="F7" s="10">
         <v>6.2</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="N7" s="2" t="e">
         <f ca="1">_xludf.CONCAT(M7,M8)</f>
@@ -4752,29 +4344,29 @@
       <c r="T7" s="2"/>
     </row>
     <row r="8" spans="1:20" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="B8" s="182" t="s">
-        <v>167</v>
-      </c>
-      <c r="C8" s="145"/>
-      <c r="D8" s="145"/>
+      <c r="B8" s="150" t="s">
+        <v>149</v>
+      </c>
+      <c r="C8" s="123"/>
+      <c r="D8" s="123"/>
       <c r="G8" s="4"/>
       <c r="H8" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="L8" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="I8" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>171</v>
-      </c>
       <c r="M8" s="8" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
@@ -4820,56 +4412,56 @@
       <c r="M12" s="11"/>
     </row>
     <row r="13" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B13" s="183"/>
-      <c r="C13" s="145"/>
-      <c r="D13" s="145"/>
+      <c r="B13" s="151"/>
+      <c r="C13" s="123"/>
+      <c r="D13" s="123"/>
       <c r="G13" s="10"/>
       <c r="H13" s="4" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="182" t="s">
-        <v>179</v>
-      </c>
-      <c r="C14" s="145"/>
-      <c r="D14" s="145"/>
+      <c r="B14" s="150" t="s">
+        <v>161</v>
+      </c>
+      <c r="C14" s="123"/>
+      <c r="D14" s="123"/>
       <c r="F14" s="10">
         <v>3.1</v>
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="5" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
       <c r="N14" s="2" t="e">
         <f ca="1">_xludf.CONCAT(M14,M15)</f>
@@ -4899,25 +4491,25 @@
     <row r="15" spans="1:20" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="13"/>
       <c r="G15" s="12" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
@@ -4939,32 +4531,32 @@
       <c r="M17" s="4"/>
     </row>
     <row r="18" spans="2:19" ht="255" x14ac:dyDescent="0.2">
-      <c r="B18" s="182" t="s">
-        <v>191</v>
-      </c>
-      <c r="C18" s="145"/>
-      <c r="D18" s="145"/>
+      <c r="B18" s="150" t="s">
+        <v>173</v>
+      </c>
+      <c r="C18" s="123"/>
+      <c r="D18" s="123"/>
       <c r="F18" s="10">
         <v>3.2</v>
       </c>
       <c r="G18" s="10"/>
       <c r="H18" s="5" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="N18" s="4" t="e">
         <f ca="1">_xludf.CONCAT(M18,M19)</f>
@@ -4994,15 +4586,15 @@
     <row r="19" spans="2:19" ht="127.5" x14ac:dyDescent="0.2">
       <c r="G19" s="10"/>
       <c r="H19" s="9" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="M19" s="4"/>
     </row>
@@ -5035,55 +4627,55 @@
     </row>
     <row r="24" spans="2:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="H24" s="10" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="K24" s="10" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="L24" s="10" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="M24" s="10" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25" spans="2:19" ht="280.5" x14ac:dyDescent="0.2">
-      <c r="B25" s="183" t="s">
-        <v>203</v>
-      </c>
-      <c r="C25" s="145"/>
-      <c r="D25" s="145"/>
+      <c r="B25" s="151" t="s">
+        <v>185</v>
+      </c>
+      <c r="C25" s="123"/>
+      <c r="D25" s="123"/>
       <c r="G25" s="10" t="s">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
     </row>
     <row r="26" spans="2:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G26" s="10" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -5103,21 +4695,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010064DEF28CA2629948A9F801C782641252" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5d88cf87ad5ac9fc8fb83d77fe1635d4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bd38d267-56bb-4e22-b975-199a06fd69fa" xmlns:ns3="d8c712e5-67fc-4595-93cb-a4164dd8eff3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1d44111b7d9e9f445610cec830697d19" ns2:_="" ns3:_="">
     <xsd:import namespace="bd38d267-56bb-4e22-b975-199a06fd69fa"/>
@@ -5332,32 +4915,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BB72468-B9EB-412A-8D55-6151E9A308C0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D98D897-3D5D-4CF5-A274-8B2E15AE73B2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="bd38d267-56bb-4e22-b975-199a06fd69fa"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="d8c712e5-67fc-4595-93cb-a4164dd8eff3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D98D897-3D5D-4CF5-A274-8B2E15AE73B2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="bd38d267-56bb-4e22-b975-199a06fd69fa"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="d8c712e5-67fc-4595-93cb-a4164dd8eff3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A22DEBAC-93F7-4736-A2B9-33A782348601}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5374,4 +4958,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BB72468-B9EB-412A-8D55-6151E9A308C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Y2A - Minor Spelling fixes in assement rubric and readme
</commit_message>
<xml_diff>
--- a/docs/Year2/BlockA/MS Teams Assignment Template/2022-23 ADS&AI Assessment Rubric Y2A.xlsx
+++ b/docs/Year2/BlockA/MS Teams Assignment Template/2022-23 ADS&AI Assessment Rubric Y2A.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bramh\Documents\GitHub\AAI-DM\docs\Year2\BlockA\MS Teams Assignment Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A8EE8B-B913-4B92-9660-E44E3AD53F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74B8302-555C-4E52-9FE0-DDA315F51DBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="50910" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51480" yWindow="3495" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Student Self-Assessment" sheetId="6" r:id="rId1"/>
@@ -194,9 +194,6 @@
     <t xml:space="preserve">Clear comments per submission. All docementation required is present. Submissions are thouroughly checked before submitting.  Clear understanding of workspaces/client/server. And meeting all criteria in insufficient. </t>
   </si>
   <si>
-    <t xml:space="preserve">Each submission clearly demonstrates clear processing of feedback recieved. Correct spelling and good grammar used. Use of professional wording throughout. And meeting all criteria in sufficient. </t>
-  </si>
-  <si>
     <t>2.0 Personal Development &amp; Academic Practice
 The student demonstrate self-exploration and personal development, good academic practices in learning how to learn and the acquisition of professional knowledge through research, 
 study, analysis, applied practice, discussion and reporting, where an excellent performance would show:</t>
@@ -224,43 +221,7 @@
     <t>1,2</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>3.0 Digital Transformation 2:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> The student is able to explain and contrast the attitudes, knowledge, acceptance, and perceived impact of AI on the domains of Buas by means of a research proposal and formulate research questions and consequently, hypotheses which can be tested.​</t>
-    </r>
-  </si>
-  <si>
-    <t>The student is able to explore and contrast the attitudes, knowledge, acceptance, and perceived impact of AI on the domains of Buas by means of a literature study and on this basis, draft a research proposal formulating research questions and consequently, hypotheses which can be tested.​</t>
-  </si>
-  <si>
     <t>The student attends the mini-conference.</t>
-  </si>
-  <si>
-    <t>A literature review documenting the current state of attitudes, knowledge, acceptance, and percieved impact of AI on the domains of Buas is present.  And meeting all criteria in poor.</t>
-  </si>
-  <si>
-    <t>Research question(s) investigating the current state of attitudes, knowledge, acceptance, and percieved impact of AI on the domains of Buas are formulated. And meeting all criteria in insufficient.</t>
-  </si>
-  <si>
-    <t>Research questions investigating the current state of attitudes, knowledge, acceptance, and percieved impact of AI on the domains of Buas are translated into hypothesis which can be put to the test. And meeting all criteria in sufficient.</t>
-  </si>
-  <si>
-    <t>A coherent research proposal is present containing the current state of attitudes, knowledge, acceptance, and percieved impact of AI on the domains of Buas. And meeting all criteria in Good.</t>
   </si>
   <si>
     <r>
@@ -309,16 +270,10 @@
     <t>The student is able to develop and implement appropriate data management methods integrating legal and ethical concerns to facilitate their study design.​</t>
   </si>
   <si>
-    <t>A data management plan is present and is based on the Buas DMP template.</t>
-  </si>
-  <si>
     <t>A description of the data collection process (quantitative and qualitative) is present. And meets all criteria in poor.</t>
   </si>
   <si>
     <t>A codebook describing variables is present. And meets all criteria in insufficient.</t>
-  </si>
-  <si>
-    <t>A data storage protocol adhering to the Buas Data Management Protocol is present. And meets all criteria in sufficient.</t>
   </si>
   <si>
     <t xml:space="preserve">The data management plan ensures that the data adheres to F.A.I.R principles. And meeting all criteria in good. </t>
@@ -803,6 +758,33 @@
   </si>
   <si>
     <t>The student is able to communicate findings by means of a structured, coherent, and well argued  scientific report using Latex.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Each submission clearly demonstrates clear processing of feedback received. Correct spelling and good grammar used. Use of professional wording throughout. And meeting all criteria in sufficient. </t>
+  </si>
+  <si>
+    <t>A data management plan is present and is based on the BUas DMP template.</t>
+  </si>
+  <si>
+    <t>3.0 Digital Transformation 2: The student is able to explain and contrast the attitudes, knowledge, acceptance, and perceived impact of AI on the domains of BUas by means of a research proposal and formulate research questions and consequently, hypotheses which can be tested.​</t>
+  </si>
+  <si>
+    <t>The student is able to explore and contrast the attitudes, knowledge, acceptance, and perceived impact of AI on the domains of BUas by means of a literature study and on this basis, draft a research proposal formulating research questions and consequently, hypotheses which can be tested.​</t>
+  </si>
+  <si>
+    <t>A literature review documenting the current state of attitudes, knowledge, acceptance, and perceived impact of AI on the domains of BUas is present.  And meeting all criteria in poor.</t>
+  </si>
+  <si>
+    <t>Research question(s) investigating the current state of attitudes, knowledge, acceptance, and perceived impact of AI on the domains of BUas are formulated. And meeting all criteria in insufficient.</t>
+  </si>
+  <si>
+    <t>Research questions investigating the current state of attitudes, knowledge, acceptance, and perceived impact of AI on the domains of BUas are translated into hypothesis which can be put to the test. And meeting all criteria in sufficient.</t>
+  </si>
+  <si>
+    <t>A coherent research proposal is present containing the current state of attitudes, knowledge, acceptance, and perceived impact of AI on the domains of BUas. And meeting all criteria in Good.</t>
+  </si>
+  <si>
+    <t>A data storage protocol adhering to the BUas Data Management Protocol is present. And meets all criteria in sufficient.</t>
   </si>
 </sst>
 </file>
@@ -1570,21 +1552,107 @@
     <xf numFmtId="0" fontId="26" fillId="48" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="27" fillId="49" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1597,107 +1665,21 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2264,9 +2246,9 @@
   </sheetPr>
   <dimension ref="A1:W54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D26" sqref="D26:E26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2308,11 +2290,11 @@
     <row r="2" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="17"/>
       <c r="B2" s="18"/>
-      <c r="C2" s="102" t="s">
+      <c r="C2" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
@@ -2328,8 +2310,8 @@
     <row r="3" spans="1:16" s="23" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="19"/>
       <c r="B3" s="20"/>
-      <c r="C3" s="121"/>
-      <c r="D3" s="122"/>
+      <c r="C3" s="114"/>
+      <c r="D3" s="115"/>
       <c r="E3" s="38" t="s">
         <v>1</v>
       </c>
@@ -2339,40 +2321,40 @@
       <c r="G3" s="21"/>
       <c r="H3" s="22"/>
       <c r="I3" s="22"/>
-      <c r="J3" s="105" t="s">
+      <c r="J3" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="123"/>
-      <c r="L3" s="124" t="s">
+      <c r="K3" s="117"/>
+      <c r="L3" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="103"/>
-      <c r="N3" s="103"/>
+      <c r="M3" s="102"/>
+      <c r="N3" s="102"/>
       <c r="O3" s="20"/>
       <c r="P3" s="19"/>
     </row>
     <row r="4" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17"/>
       <c r="B4" s="24"/>
-      <c r="C4" s="125" t="s">
+      <c r="C4" s="119" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="103"/>
+      <c r="D4" s="102"/>
       <c r="E4" s="15"/>
-      <c r="F4" s="126"/>
-      <c r="G4" s="127"/>
-      <c r="H4" s="127"/>
-      <c r="I4" s="127"/>
-      <c r="J4" s="128"/>
-      <c r="K4" s="129"/>
-      <c r="L4" s="130" t="s">
+      <c r="F4" s="120"/>
+      <c r="G4" s="121"/>
+      <c r="H4" s="121"/>
+      <c r="I4" s="121"/>
+      <c r="J4" s="122"/>
+      <c r="K4" s="123"/>
+      <c r="L4" s="124" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="131">
+      <c r="M4" s="125">
         <f>IF(ROUND((N24/10),1)&lt;&gt;ROUND((N24/10),0),ROUND((N2/10),1),ROUND((N24/10),0))</f>
         <v>0</v>
       </c>
-      <c r="N4" s="132" t="str">
+      <c r="N4" s="126" t="str">
         <f>IF(M4&gt;=5.5,"PASS",IF(M4&gt;0,"FAIL","M/O"))</f>
         <v>M/O</v>
       </c>
@@ -2382,86 +2364,86 @@
     <row r="5" spans="1:16" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="17"/>
       <c r="B5" s="24"/>
-      <c r="C5" s="125" t="s">
+      <c r="C5" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="123"/>
+      <c r="D5" s="117"/>
       <c r="E5" s="15"/>
-      <c r="F5" s="127"/>
-      <c r="G5" s="127"/>
-      <c r="H5" s="127"/>
-      <c r="I5" s="127"/>
-      <c r="J5" s="129"/>
-      <c r="K5" s="129"/>
-      <c r="L5" s="123"/>
-      <c r="M5" s="123"/>
-      <c r="N5" s="123"/>
+      <c r="F5" s="121"/>
+      <c r="G5" s="121"/>
+      <c r="H5" s="121"/>
+      <c r="I5" s="121"/>
+      <c r="J5" s="123"/>
+      <c r="K5" s="123"/>
+      <c r="L5" s="117"/>
+      <c r="M5" s="117"/>
+      <c r="N5" s="117"/>
       <c r="O5" s="18"/>
       <c r="P5" s="17"/>
     </row>
     <row r="6" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="17"/>
       <c r="B6" s="24"/>
-      <c r="C6" s="125" t="s">
+      <c r="C6" s="119" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="133"/>
+      <c r="D6" s="127"/>
       <c r="E6" s="96" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="127"/>
-      <c r="G6" s="127"/>
-      <c r="H6" s="127"/>
-      <c r="I6" s="127"/>
-      <c r="J6" s="129"/>
-      <c r="K6" s="129"/>
-      <c r="L6" s="123"/>
-      <c r="M6" s="123"/>
-      <c r="N6" s="123"/>
+      <c r="F6" s="121"/>
+      <c r="G6" s="121"/>
+      <c r="H6" s="121"/>
+      <c r="I6" s="121"/>
+      <c r="J6" s="123"/>
+      <c r="K6" s="123"/>
+      <c r="L6" s="117"/>
+      <c r="M6" s="117"/>
+      <c r="N6" s="117"/>
       <c r="O6" s="18"/>
       <c r="P6" s="17"/>
     </row>
     <row r="7" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="17"/>
       <c r="B7" s="24"/>
-      <c r="C7" s="125" t="s">
+      <c r="C7" s="119" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="123"/>
+      <c r="D7" s="117"/>
       <c r="E7" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="127"/>
-      <c r="G7" s="127"/>
-      <c r="H7" s="127"/>
-      <c r="I7" s="127"/>
-      <c r="J7" s="129"/>
-      <c r="K7" s="129"/>
-      <c r="L7" s="123"/>
-      <c r="M7" s="123"/>
-      <c r="N7" s="123"/>
+      <c r="F7" s="121"/>
+      <c r="G7" s="121"/>
+      <c r="H7" s="121"/>
+      <c r="I7" s="121"/>
+      <c r="J7" s="123"/>
+      <c r="K7" s="123"/>
+      <c r="L7" s="117"/>
+      <c r="M7" s="117"/>
+      <c r="N7" s="117"/>
       <c r="O7" s="18"/>
       <c r="P7" s="17"/>
     </row>
     <row r="8" spans="1:16" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17"/>
       <c r="B8" s="24"/>
-      <c r="C8" s="134" t="s">
+      <c r="C8" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="135"/>
+      <c r="D8" s="129"/>
       <c r="E8" s="40" t="s">
-        <v>194</v>
-      </c>
-      <c r="F8" s="127"/>
-      <c r="G8" s="127"/>
-      <c r="H8" s="127"/>
-      <c r="I8" s="127"/>
-      <c r="J8" s="129"/>
-      <c r="K8" s="129"/>
-      <c r="L8" s="123"/>
-      <c r="M8" s="123"/>
-      <c r="N8" s="123"/>
+        <v>185</v>
+      </c>
+      <c r="F8" s="121"/>
+      <c r="G8" s="121"/>
+      <c r="H8" s="121"/>
+      <c r="I8" s="121"/>
+      <c r="J8" s="123"/>
+      <c r="K8" s="123"/>
+      <c r="L8" s="117"/>
+      <c r="M8" s="117"/>
+      <c r="N8" s="117"/>
       <c r="O8" s="18"/>
       <c r="P8" s="17"/>
     </row>
@@ -2504,11 +2486,11 @@
     <row r="11" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A11" s="17"/>
       <c r="B11" s="18"/>
-      <c r="C11" s="102" t="s">
+      <c r="C11" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="103"/>
-      <c r="E11" s="103"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="102"/>
       <c r="F11" s="18"/>
       <c r="G11" s="18"/>
       <c r="H11" s="18"/>
@@ -2525,7 +2507,7 @@
       <c r="A12" s="17"/>
       <c r="B12" s="18"/>
       <c r="C12" s="43" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="D12" s="44" t="s">
         <v>14</v>
@@ -2564,19 +2546,19 @@
     <row r="13" spans="1:16" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="17"/>
       <c r="B13" s="27"/>
-      <c r="C13" s="136">
+      <c r="C13" s="103">
         <v>9</v>
       </c>
-      <c r="D13" s="144" t="s">
+      <c r="D13" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="144"/>
-      <c r="F13" s="144"/>
-      <c r="G13" s="144"/>
-      <c r="H13" s="144"/>
-      <c r="I13" s="144"/>
-      <c r="J13" s="144"/>
-      <c r="K13" s="144"/>
+      <c r="E13" s="104"/>
+      <c r="F13" s="104"/>
+      <c r="G13" s="104"/>
+      <c r="H13" s="104"/>
+      <c r="I13" s="104"/>
+      <c r="J13" s="104"/>
+      <c r="K13" s="104"/>
       <c r="L13" s="82"/>
       <c r="M13" s="82"/>
       <c r="N13" s="82"/>
@@ -2586,11 +2568,11 @@
     <row r="14" spans="1:16" ht="118.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="17"/>
       <c r="B14" s="18"/>
-      <c r="C14" s="136"/>
-      <c r="D14" s="145" t="s">
+      <c r="C14" s="103"/>
+      <c r="D14" s="105" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="145"/>
+      <c r="E14" s="105"/>
       <c r="F14" s="81" t="s">
         <v>26</v>
       </c>
@@ -2604,10 +2586,10 @@
         <v>29</v>
       </c>
       <c r="J14" s="54" t="s">
-        <v>30</v>
+        <v>199</v>
       </c>
       <c r="K14" s="55" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="L14" s="42">
         <v>10</v>
@@ -2626,16 +2608,16 @@
       <c r="A15" s="17"/>
       <c r="B15" s="27"/>
       <c r="C15" s="95"/>
-      <c r="D15" s="146" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="139"/>
-      <c r="F15" s="139"/>
-      <c r="G15" s="139"/>
-      <c r="H15" s="139"/>
-      <c r="I15" s="139"/>
-      <c r="J15" s="139"/>
-      <c r="K15" s="139"/>
+      <c r="D15" s="106" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="107"/>
+      <c r="F15" s="107"/>
+      <c r="G15" s="107"/>
+      <c r="H15" s="107"/>
+      <c r="I15" s="107"/>
+      <c r="J15" s="107"/>
+      <c r="K15" s="107"/>
       <c r="L15" s="83"/>
       <c r="M15" s="83"/>
       <c r="N15" s="83"/>
@@ -2646,29 +2628,29 @@
       <c r="A16" s="17"/>
       <c r="B16" s="18"/>
       <c r="C16" s="95" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="99" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="119" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="140"/>
+      <c r="E16" s="100"/>
       <c r="F16" s="81" t="s">
         <v>26</v>
       </c>
       <c r="G16" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="H16" s="52" t="s">
+      <c r="I16" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="I16" s="53" t="s">
+      <c r="J16" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="J16" s="54" t="s">
-        <v>37</v>
-      </c>
       <c r="K16" s="55" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="L16" s="42">
         <v>10</v>
@@ -2686,19 +2668,19 @@
     <row r="17" spans="1:23" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="17"/>
       <c r="B17" s="27"/>
-      <c r="C17" s="138" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="139" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="139"/>
-      <c r="F17" s="139"/>
-      <c r="G17" s="139"/>
-      <c r="H17" s="139"/>
-      <c r="I17" s="139"/>
-      <c r="J17" s="139"/>
-      <c r="K17" s="139"/>
+      <c r="C17" s="110" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="107" t="s">
+        <v>201</v>
+      </c>
+      <c r="E17" s="107"/>
+      <c r="F17" s="107"/>
+      <c r="G17" s="107"/>
+      <c r="H17" s="107"/>
+      <c r="I17" s="107"/>
+      <c r="J17" s="107"/>
+      <c r="K17" s="107"/>
       <c r="L17" s="83"/>
       <c r="M17" s="83"/>
       <c r="N17" s="83"/>
@@ -2715,28 +2697,28 @@
     <row r="18" spans="1:23" ht="111.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="17"/>
       <c r="B18" s="18"/>
-      <c r="C18" s="138"/>
-      <c r="D18" s="119" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="140"/>
+      <c r="C18" s="110"/>
+      <c r="D18" s="99" t="s">
+        <v>202</v>
+      </c>
+      <c r="E18" s="100"/>
       <c r="F18" s="81" t="s">
         <v>26</v>
       </c>
       <c r="G18" s="51" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H18" s="52" t="s">
-        <v>42</v>
+        <v>203</v>
       </c>
       <c r="I18" s="53" t="s">
-        <v>43</v>
+        <v>204</v>
       </c>
       <c r="J18" s="54" t="s">
-        <v>44</v>
+        <v>205</v>
       </c>
       <c r="K18" s="55" t="s">
-        <v>45</v>
+        <v>206</v>
       </c>
       <c r="L18" s="42">
         <v>10</v>
@@ -2761,19 +2743,19 @@
     <row r="19" spans="1:23" ht="42.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="17"/>
       <c r="B19" s="27"/>
-      <c r="C19" s="136">
+      <c r="C19" s="103">
         <v>3</v>
       </c>
-      <c r="D19" s="141" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="142"/>
-      <c r="F19" s="142"/>
-      <c r="G19" s="142"/>
-      <c r="H19" s="142"/>
-      <c r="I19" s="142"/>
-      <c r="J19" s="142"/>
-      <c r="K19" s="142"/>
+      <c r="D19" s="111" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="112"/>
+      <c r="F19" s="112"/>
+      <c r="G19" s="112"/>
+      <c r="H19" s="112"/>
+      <c r="I19" s="112"/>
+      <c r="J19" s="112"/>
+      <c r="K19" s="112"/>
       <c r="L19" s="46"/>
       <c r="M19" s="46"/>
       <c r="N19" s="46"/>
@@ -2790,28 +2772,28 @@
     <row r="20" spans="1:23" s="57" customFormat="1" ht="111.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="49"/>
       <c r="B20" s="50"/>
-      <c r="C20" s="103"/>
-      <c r="D20" s="143" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" s="143"/>
+      <c r="C20" s="102"/>
+      <c r="D20" s="113" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="113"/>
       <c r="F20" s="81" t="s">
         <v>26</v>
       </c>
       <c r="G20" s="60" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="H20" s="61" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="I20" s="62" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="J20" s="63" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="K20" s="64" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="L20" s="42">
         <v>15</v>
@@ -2836,17 +2818,17 @@
     <row r="21" spans="1:23" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="17"/>
       <c r="B21" s="18"/>
-      <c r="C21" s="136" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="137" t="s">
-        <v>52</v>
-      </c>
-      <c r="E21" s="118"/>
-      <c r="F21" s="118"/>
-      <c r="G21" s="118"/>
-      <c r="H21" s="118"/>
-      <c r="I21" s="118"/>
+      <c r="C21" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="108" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="109"/>
+      <c r="F21" s="109"/>
+      <c r="G21" s="109"/>
+      <c r="H21" s="109"/>
+      <c r="I21" s="109"/>
       <c r="J21" s="86"/>
       <c r="K21" s="86"/>
       <c r="L21" s="83"/>
@@ -2865,28 +2847,28 @@
     <row r="22" spans="1:23" ht="138.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17"/>
       <c r="B22" s="18"/>
-      <c r="C22" s="103"/>
-      <c r="D22" s="119" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22" s="119"/>
+      <c r="C22" s="102"/>
+      <c r="D22" s="99" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="99"/>
       <c r="F22" s="81" t="s">
         <v>26</v>
       </c>
       <c r="G22" s="58" t="s">
-        <v>54</v>
+        <v>200</v>
       </c>
       <c r="H22" s="41" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="I22" s="47" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="J22" s="63" t="s">
-        <v>57</v>
+        <v>207</v>
       </c>
       <c r="K22" s="48" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="L22" s="42">
         <v>15</v>
@@ -2912,14 +2894,14 @@
       <c r="A23" s="17"/>
       <c r="B23" s="18"/>
       <c r="C23" s="59"/>
-      <c r="D23" s="118" t="s">
-        <v>59</v>
-      </c>
-      <c r="E23" s="118"/>
-      <c r="F23" s="118"/>
-      <c r="G23" s="118"/>
-      <c r="H23" s="118"/>
-      <c r="I23" s="118"/>
+      <c r="D23" s="109" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="109"/>
+      <c r="F23" s="109"/>
+      <c r="G23" s="109"/>
+      <c r="H23" s="109"/>
+      <c r="I23" s="109"/>
       <c r="J23" s="86"/>
       <c r="K23" s="86"/>
       <c r="L23" s="83"/>
@@ -2939,29 +2921,29 @@
       <c r="A24" s="17"/>
       <c r="B24" s="18"/>
       <c r="C24" s="59" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" s="119" t="s">
-        <v>61</v>
-      </c>
-      <c r="E24" s="119"/>
+        <v>51</v>
+      </c>
+      <c r="D24" s="99" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="99"/>
       <c r="F24" s="81" t="s">
         <v>26</v>
       </c>
       <c r="G24" s="58" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="H24" s="41" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="I24" s="47" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="J24" s="63" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="K24" s="48" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="L24" s="42">
         <v>20</v>
@@ -2987,14 +2969,14 @@
       <c r="A25" s="17"/>
       <c r="B25" s="18"/>
       <c r="C25" s="59"/>
-      <c r="D25" s="118" t="s">
-        <v>206</v>
-      </c>
-      <c r="E25" s="118"/>
-      <c r="F25" s="118"/>
-      <c r="G25" s="118"/>
-      <c r="H25" s="118"/>
-      <c r="I25" s="118"/>
+      <c r="D25" s="109" t="s">
+        <v>197</v>
+      </c>
+      <c r="E25" s="109"/>
+      <c r="F25" s="109"/>
+      <c r="G25" s="109"/>
+      <c r="H25" s="109"/>
+      <c r="I25" s="109"/>
       <c r="J25" s="86"/>
       <c r="K25" s="86"/>
       <c r="L25" s="83"/>
@@ -3014,29 +2996,29 @@
       <c r="A26" s="17"/>
       <c r="B26" s="18"/>
       <c r="C26" s="59" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" s="119" t="s">
-        <v>207</v>
-      </c>
-      <c r="E26" s="119"/>
+        <v>51</v>
+      </c>
+      <c r="D26" s="99" t="s">
+        <v>198</v>
+      </c>
+      <c r="E26" s="99"/>
       <c r="F26" s="81" t="s">
         <v>26</v>
       </c>
       <c r="G26" s="58" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="H26" s="41" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="I26" s="47" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="J26" s="63" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="K26" s="48" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="L26" s="42">
         <v>20</v>
@@ -3070,14 +3052,14 @@
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
       <c r="K27" s="97" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="L27" s="97">
         <f>SUM(L14,L16,L18,L20,L22,L24,L26)</f>
         <v>100</v>
       </c>
       <c r="M27" s="98" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="N27" s="98">
         <f>SUM(N14,N16,N18,N20,N22,N24,N26)</f>
@@ -3114,11 +3096,11 @@
     <row r="29" spans="1:23" s="59" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A29" s="17"/>
       <c r="B29" s="29"/>
-      <c r="C29" s="102" t="s">
-        <v>72</v>
-      </c>
-      <c r="D29" s="103"/>
-      <c r="E29" s="103"/>
+      <c r="C29" s="101" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="102"/>
+      <c r="E29" s="102"/>
       <c r="F29" s="29"/>
       <c r="G29" s="29"/>
       <c r="H29" s="29"/>
@@ -3135,26 +3117,26 @@
       <c r="A30" s="17"/>
       <c r="B30" s="29"/>
       <c r="C30" s="89" t="s">
-        <v>73</v>
-      </c>
-      <c r="D30" s="105" t="s">
-        <v>74</v>
-      </c>
-      <c r="E30" s="103"/>
+        <v>64</v>
+      </c>
+      <c r="D30" s="116" t="s">
+        <v>65</v>
+      </c>
+      <c r="E30" s="102"/>
       <c r="F30" s="89" t="s">
-        <v>75</v>
-      </c>
-      <c r="G30" s="105" t="s">
+        <v>66</v>
+      </c>
+      <c r="G30" s="116" t="s">
         <v>2</v>
       </c>
-      <c r="H30" s="103"/>
-      <c r="I30" s="103"/>
-      <c r="J30" s="103"/>
-      <c r="K30" s="103"/>
+      <c r="H30" s="102"/>
+      <c r="I30" s="102"/>
+      <c r="J30" s="102"/>
+      <c r="K30" s="102"/>
       <c r="L30" s="65"/>
       <c r="M30" s="89"/>
       <c r="N30" s="92" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="O30" s="29"/>
       <c r="P30" s="17"/>
@@ -3165,22 +3147,22 @@
       <c r="C31" s="66">
         <v>9</v>
       </c>
-      <c r="D31" s="115" t="s">
-        <v>77</v>
-      </c>
-      <c r="E31" s="116"/>
+      <c r="D31" s="133" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" s="131"/>
       <c r="F31" s="91" t="s">
-        <v>78</v>
-      </c>
-      <c r="G31" s="117" t="s">
-        <v>79</v>
-      </c>
-      <c r="H31" s="117"/>
-      <c r="I31" s="117"/>
-      <c r="J31" s="117"/>
-      <c r="K31" s="117"/>
-      <c r="L31" s="117"/>
-      <c r="M31" s="117"/>
+        <v>69</v>
+      </c>
+      <c r="G31" s="132" t="s">
+        <v>70</v>
+      </c>
+      <c r="H31" s="132"/>
+      <c r="I31" s="132"/>
+      <c r="J31" s="132"/>
+      <c r="K31" s="132"/>
+      <c r="L31" s="132"/>
+      <c r="M31" s="132"/>
       <c r="N31" s="67">
         <v>3</v>
       </c>
@@ -3193,22 +3175,22 @@
       <c r="C32" s="68">
         <v>10</v>
       </c>
-      <c r="D32" s="120" t="s">
-        <v>77</v>
-      </c>
-      <c r="E32" s="116"/>
+      <c r="D32" s="130" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32" s="131"/>
       <c r="F32" s="91" t="s">
-        <v>80</v>
-      </c>
-      <c r="G32" s="117" t="s">
-        <v>81</v>
-      </c>
-      <c r="H32" s="117"/>
-      <c r="I32" s="117"/>
-      <c r="J32" s="117"/>
-      <c r="K32" s="117"/>
-      <c r="L32" s="117"/>
-      <c r="M32" s="117"/>
+        <v>71</v>
+      </c>
+      <c r="G32" s="132" t="s">
+        <v>72</v>
+      </c>
+      <c r="H32" s="132"/>
+      <c r="I32" s="132"/>
+      <c r="J32" s="132"/>
+      <c r="K32" s="132"/>
+      <c r="L32" s="132"/>
+      <c r="M32" s="132"/>
       <c r="N32" s="69">
         <v>3</v>
       </c>
@@ -3221,22 +3203,22 @@
       <c r="C33" s="66">
         <v>11</v>
       </c>
-      <c r="D33" s="115" t="s">
-        <v>77</v>
-      </c>
-      <c r="E33" s="116"/>
+      <c r="D33" s="133" t="s">
+        <v>68</v>
+      </c>
+      <c r="E33" s="131"/>
       <c r="F33" s="91" t="s">
-        <v>82</v>
-      </c>
-      <c r="G33" s="117" t="s">
-        <v>83</v>
-      </c>
-      <c r="H33" s="117"/>
-      <c r="I33" s="117"/>
-      <c r="J33" s="117"/>
-      <c r="K33" s="117"/>
-      <c r="L33" s="117"/>
-      <c r="M33" s="117"/>
+        <v>73</v>
+      </c>
+      <c r="G33" s="132" t="s">
+        <v>74</v>
+      </c>
+      <c r="H33" s="132"/>
+      <c r="I33" s="132"/>
+      <c r="J33" s="132"/>
+      <c r="K33" s="132"/>
+      <c r="L33" s="132"/>
+      <c r="M33" s="132"/>
       <c r="N33" s="67">
         <v>3</v>
       </c>
@@ -3249,22 +3231,22 @@
       <c r="C34" s="70">
         <v>1</v>
       </c>
-      <c r="D34" s="113" t="s">
-        <v>84</v>
-      </c>
-      <c r="E34" s="113"/>
+      <c r="D34" s="134" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" s="134"/>
       <c r="F34" s="90" t="s">
-        <v>85</v>
-      </c>
-      <c r="G34" s="111" t="s">
-        <v>205</v>
-      </c>
-      <c r="H34" s="111"/>
-      <c r="I34" s="111"/>
-      <c r="J34" s="111"/>
-      <c r="K34" s="111"/>
-      <c r="L34" s="111"/>
-      <c r="M34" s="111"/>
+        <v>76</v>
+      </c>
+      <c r="G34" s="135" t="s">
+        <v>196</v>
+      </c>
+      <c r="H34" s="135"/>
+      <c r="I34" s="135"/>
+      <c r="J34" s="135"/>
+      <c r="K34" s="135"/>
+      <c r="L34" s="135"/>
+      <c r="M34" s="135"/>
       <c r="N34" s="71">
         <v>3</v>
       </c>
@@ -3277,22 +3259,22 @@
       <c r="C35" s="72">
         <v>2</v>
       </c>
-      <c r="D35" s="106" t="s">
-        <v>84</v>
-      </c>
-      <c r="E35" s="107"/>
+      <c r="D35" s="136" t="s">
+        <v>75</v>
+      </c>
+      <c r="E35" s="137"/>
       <c r="F35" s="87" t="s">
-        <v>86</v>
-      </c>
-      <c r="G35" s="108" t="s">
-        <v>87</v>
-      </c>
-      <c r="H35" s="108"/>
-      <c r="I35" s="108"/>
-      <c r="J35" s="108"/>
-      <c r="K35" s="108"/>
-      <c r="L35" s="108"/>
-      <c r="M35" s="108"/>
+        <v>77</v>
+      </c>
+      <c r="G35" s="138" t="s">
+        <v>78</v>
+      </c>
+      <c r="H35" s="138"/>
+      <c r="I35" s="138"/>
+      <c r="J35" s="138"/>
+      <c r="K35" s="138"/>
+      <c r="L35" s="138"/>
+      <c r="M35" s="138"/>
       <c r="N35" s="73">
         <v>3</v>
       </c>
@@ -3305,22 +3287,22 @@
       <c r="C36" s="74">
         <v>3</v>
       </c>
-      <c r="D36" s="109" t="s">
-        <v>88</v>
-      </c>
-      <c r="E36" s="110"/>
+      <c r="D36" s="139" t="s">
+        <v>79</v>
+      </c>
+      <c r="E36" s="140"/>
       <c r="F36" s="90" t="s">
-        <v>89</v>
-      </c>
-      <c r="G36" s="111" t="s">
-        <v>90</v>
-      </c>
-      <c r="H36" s="111"/>
-      <c r="I36" s="111"/>
-      <c r="J36" s="111"/>
-      <c r="K36" s="111"/>
-      <c r="L36" s="111"/>
-      <c r="M36" s="111"/>
+        <v>80</v>
+      </c>
+      <c r="G36" s="135" t="s">
+        <v>81</v>
+      </c>
+      <c r="H36" s="135"/>
+      <c r="I36" s="135"/>
+      <c r="J36" s="135"/>
+      <c r="K36" s="135"/>
+      <c r="L36" s="135"/>
+      <c r="M36" s="135"/>
       <c r="N36" s="75">
         <v>3</v>
       </c>
@@ -3333,22 +3315,22 @@
       <c r="C37" s="76">
         <v>4</v>
       </c>
-      <c r="D37" s="112" t="s">
-        <v>91</v>
-      </c>
-      <c r="E37" s="107"/>
+      <c r="D37" s="141" t="s">
+        <v>82</v>
+      </c>
+      <c r="E37" s="137"/>
       <c r="F37" s="87" t="s">
-        <v>92</v>
-      </c>
-      <c r="G37" s="108" t="s">
-        <v>202</v>
-      </c>
-      <c r="H37" s="108"/>
-      <c r="I37" s="108"/>
-      <c r="J37" s="108"/>
-      <c r="K37" s="108"/>
-      <c r="L37" s="108"/>
-      <c r="M37" s="108"/>
+        <v>83</v>
+      </c>
+      <c r="G37" s="138" t="s">
+        <v>193</v>
+      </c>
+      <c r="H37" s="138"/>
+      <c r="I37" s="138"/>
+      <c r="J37" s="138"/>
+      <c r="K37" s="138"/>
+      <c r="L37" s="138"/>
+      <c r="M37" s="138"/>
       <c r="N37" s="77">
         <v>3</v>
       </c>
@@ -3361,22 +3343,22 @@
       <c r="C38" s="70">
         <v>5</v>
       </c>
-      <c r="D38" s="113" t="s">
-        <v>93</v>
-      </c>
-      <c r="E38" s="114"/>
+      <c r="D38" s="134" t="s">
+        <v>84</v>
+      </c>
+      <c r="E38" s="142"/>
       <c r="F38" s="90" t="s">
-        <v>93</v>
-      </c>
-      <c r="G38" s="111" t="s">
-        <v>203</v>
-      </c>
-      <c r="H38" s="111"/>
-      <c r="I38" s="111"/>
-      <c r="J38" s="111"/>
-      <c r="K38" s="111"/>
-      <c r="L38" s="111"/>
-      <c r="M38" s="111"/>
+        <v>84</v>
+      </c>
+      <c r="G38" s="135" t="s">
+        <v>194</v>
+      </c>
+      <c r="H38" s="135"/>
+      <c r="I38" s="135"/>
+      <c r="J38" s="135"/>
+      <c r="K38" s="135"/>
+      <c r="L38" s="135"/>
+      <c r="M38" s="135"/>
       <c r="N38" s="71">
         <v>3</v>
       </c>
@@ -3389,22 +3371,22 @@
       <c r="C39" s="72">
         <v>6</v>
       </c>
-      <c r="D39" s="106" t="s">
-        <v>93</v>
-      </c>
-      <c r="E39" s="107"/>
+      <c r="D39" s="136" t="s">
+        <v>84</v>
+      </c>
+      <c r="E39" s="137"/>
       <c r="F39" s="87" t="s">
-        <v>94</v>
-      </c>
-      <c r="G39" s="108" t="s">
-        <v>204</v>
-      </c>
-      <c r="H39" s="108"/>
-      <c r="I39" s="108"/>
-      <c r="J39" s="108"/>
-      <c r="K39" s="108"/>
-      <c r="L39" s="108"/>
-      <c r="M39" s="108"/>
+        <v>85</v>
+      </c>
+      <c r="G39" s="138" t="s">
+        <v>195</v>
+      </c>
+      <c r="H39" s="138"/>
+      <c r="I39" s="138"/>
+      <c r="J39" s="138"/>
+      <c r="K39" s="138"/>
+      <c r="L39" s="138"/>
+      <c r="M39" s="138"/>
       <c r="N39" s="73">
         <v>3</v>
       </c>
@@ -3417,22 +3399,22 @@
       <c r="C40" s="74">
         <v>7</v>
       </c>
-      <c r="D40" s="109" t="s">
-        <v>95</v>
-      </c>
-      <c r="E40" s="110"/>
+      <c r="D40" s="139" t="s">
+        <v>86</v>
+      </c>
+      <c r="E40" s="140"/>
       <c r="F40" s="90" t="s">
-        <v>96</v>
-      </c>
-      <c r="G40" s="111" t="s">
-        <v>97</v>
-      </c>
-      <c r="H40" s="111"/>
-      <c r="I40" s="111"/>
-      <c r="J40" s="111"/>
-      <c r="K40" s="111"/>
-      <c r="L40" s="111"/>
-      <c r="M40" s="111"/>
+        <v>87</v>
+      </c>
+      <c r="G40" s="135" t="s">
+        <v>88</v>
+      </c>
+      <c r="H40" s="135"/>
+      <c r="I40" s="135"/>
+      <c r="J40" s="135"/>
+      <c r="K40" s="135"/>
+      <c r="L40" s="135"/>
+      <c r="M40" s="135"/>
       <c r="N40" s="75">
         <v>3</v>
       </c>
@@ -3445,22 +3427,22 @@
       <c r="C41" s="76">
         <v>8</v>
       </c>
-      <c r="D41" s="112" t="s">
-        <v>95</v>
-      </c>
-      <c r="E41" s="107"/>
+      <c r="D41" s="141" t="s">
+        <v>86</v>
+      </c>
+      <c r="E41" s="137"/>
       <c r="F41" s="87" t="s">
-        <v>98</v>
-      </c>
-      <c r="G41" s="108" t="s">
-        <v>99</v>
-      </c>
-      <c r="H41" s="108"/>
-      <c r="I41" s="108"/>
-      <c r="J41" s="108"/>
-      <c r="K41" s="108"/>
-      <c r="L41" s="108"/>
-      <c r="M41" s="108"/>
+        <v>89</v>
+      </c>
+      <c r="G41" s="138" t="s">
+        <v>90</v>
+      </c>
+      <c r="H41" s="138"/>
+      <c r="I41" s="138"/>
+      <c r="J41" s="138"/>
+      <c r="K41" s="138"/>
+      <c r="L41" s="138"/>
+      <c r="M41" s="138"/>
       <c r="N41" s="77">
         <v>3</v>
       </c>
@@ -3506,11 +3488,11 @@
     <row r="44" spans="1:16" s="59" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A44" s="17"/>
       <c r="B44" s="32"/>
-      <c r="C44" s="102" t="s">
-        <v>100</v>
-      </c>
-      <c r="D44" s="103"/>
-      <c r="E44" s="103"/>
+      <c r="C44" s="101" t="s">
+        <v>91</v>
+      </c>
+      <c r="D44" s="102"/>
+      <c r="E44" s="102"/>
       <c r="F44" s="27"/>
       <c r="G44" s="18"/>
       <c r="H44" s="18"/>
@@ -3527,25 +3509,25 @@
       <c r="A45" s="17"/>
       <c r="B45" s="32"/>
       <c r="C45" s="33" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D45" s="33" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="E45" s="88"/>
-      <c r="F45" s="104" t="s">
-        <v>102</v>
-      </c>
-      <c r="G45" s="103"/>
-      <c r="H45" s="103"/>
-      <c r="I45" s="103"/>
-      <c r="J45" s="105" t="s">
-        <v>103</v>
-      </c>
-      <c r="K45" s="103"/>
-      <c r="L45" s="103"/>
-      <c r="M45" s="103"/>
-      <c r="N45" s="103"/>
+      <c r="F45" s="143" t="s">
+        <v>93</v>
+      </c>
+      <c r="G45" s="102"/>
+      <c r="H45" s="102"/>
+      <c r="I45" s="102"/>
+      <c r="J45" s="116" t="s">
+        <v>94</v>
+      </c>
+      <c r="K45" s="102"/>
+      <c r="L45" s="102"/>
+      <c r="M45" s="102"/>
+      <c r="N45" s="102"/>
       <c r="O45" s="18"/>
       <c r="P45" s="17"/>
     </row>
@@ -3556,22 +3538,22 @@
         <v>1</v>
       </c>
       <c r="D46" s="36" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E46" s="85"/>
-      <c r="F46" s="99" t="s">
-        <v>105</v>
-      </c>
-      <c r="G46" s="100"/>
-      <c r="H46" s="100"/>
-      <c r="I46" s="100"/>
-      <c r="J46" s="99" t="s">
-        <v>106</v>
-      </c>
-      <c r="K46" s="100"/>
-      <c r="L46" s="100"/>
-      <c r="M46" s="100"/>
-      <c r="N46" s="100"/>
+      <c r="F46" s="146" t="s">
+        <v>96</v>
+      </c>
+      <c r="G46" s="145"/>
+      <c r="H46" s="145"/>
+      <c r="I46" s="145"/>
+      <c r="J46" s="146" t="s">
+        <v>97</v>
+      </c>
+      <c r="K46" s="145"/>
+      <c r="L46" s="145"/>
+      <c r="M46" s="145"/>
+      <c r="N46" s="145"/>
       <c r="O46" s="18"/>
       <c r="P46" s="17"/>
     </row>
@@ -3582,22 +3564,22 @@
         <v>2</v>
       </c>
       <c r="D47" s="31" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E47" s="84"/>
-      <c r="F47" s="101" t="s">
-        <v>108</v>
-      </c>
-      <c r="G47" s="100"/>
-      <c r="H47" s="100"/>
-      <c r="I47" s="100"/>
-      <c r="J47" s="101" t="s">
-        <v>109</v>
-      </c>
-      <c r="K47" s="100"/>
-      <c r="L47" s="100"/>
-      <c r="M47" s="100"/>
-      <c r="N47" s="100"/>
+      <c r="F47" s="144" t="s">
+        <v>99</v>
+      </c>
+      <c r="G47" s="145"/>
+      <c r="H47" s="145"/>
+      <c r="I47" s="145"/>
+      <c r="J47" s="144" t="s">
+        <v>100</v>
+      </c>
+      <c r="K47" s="145"/>
+      <c r="L47" s="145"/>
+      <c r="M47" s="145"/>
+      <c r="N47" s="145"/>
       <c r="O47" s="18"/>
       <c r="P47" s="17"/>
     </row>
@@ -3608,22 +3590,22 @@
         <v>3</v>
       </c>
       <c r="D48" s="36" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="E48" s="85"/>
-      <c r="F48" s="99" t="s">
-        <v>111</v>
-      </c>
-      <c r="G48" s="100"/>
-      <c r="H48" s="100"/>
-      <c r="I48" s="100"/>
-      <c r="J48" s="99" t="s">
-        <v>112</v>
-      </c>
-      <c r="K48" s="100"/>
-      <c r="L48" s="100"/>
-      <c r="M48" s="100"/>
-      <c r="N48" s="100"/>
+      <c r="F48" s="146" t="s">
+        <v>102</v>
+      </c>
+      <c r="G48" s="145"/>
+      <c r="H48" s="145"/>
+      <c r="I48" s="145"/>
+      <c r="J48" s="146" t="s">
+        <v>103</v>
+      </c>
+      <c r="K48" s="145"/>
+      <c r="L48" s="145"/>
+      <c r="M48" s="145"/>
+      <c r="N48" s="145"/>
       <c r="O48" s="18"/>
       <c r="P48" s="17"/>
     </row>
@@ -3634,22 +3616,22 @@
         <v>4</v>
       </c>
       <c r="D49" s="31" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="E49" s="84"/>
-      <c r="F49" s="101" t="s">
-        <v>114</v>
-      </c>
-      <c r="G49" s="100"/>
-      <c r="H49" s="100"/>
-      <c r="I49" s="100"/>
-      <c r="J49" s="101" t="s">
-        <v>115</v>
-      </c>
-      <c r="K49" s="100"/>
-      <c r="L49" s="100"/>
-      <c r="M49" s="100"/>
-      <c r="N49" s="100"/>
+      <c r="F49" s="144" t="s">
+        <v>105</v>
+      </c>
+      <c r="G49" s="145"/>
+      <c r="H49" s="145"/>
+      <c r="I49" s="145"/>
+      <c r="J49" s="144" t="s">
+        <v>106</v>
+      </c>
+      <c r="K49" s="145"/>
+      <c r="L49" s="145"/>
+      <c r="M49" s="145"/>
+      <c r="N49" s="145"/>
       <c r="O49" s="18"/>
       <c r="P49" s="17"/>
     </row>
@@ -3660,22 +3642,22 @@
         <v>5</v>
       </c>
       <c r="D50" s="36" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="E50" s="85"/>
-      <c r="F50" s="99" t="s">
-        <v>117</v>
-      </c>
-      <c r="G50" s="100"/>
-      <c r="H50" s="100"/>
-      <c r="I50" s="100"/>
-      <c r="J50" s="99" t="s">
-        <v>118</v>
-      </c>
-      <c r="K50" s="100"/>
-      <c r="L50" s="100"/>
-      <c r="M50" s="100"/>
-      <c r="N50" s="100"/>
+      <c r="F50" s="146" t="s">
+        <v>108</v>
+      </c>
+      <c r="G50" s="145"/>
+      <c r="H50" s="145"/>
+      <c r="I50" s="145"/>
+      <c r="J50" s="146" t="s">
+        <v>109</v>
+      </c>
+      <c r="K50" s="145"/>
+      <c r="L50" s="145"/>
+      <c r="M50" s="145"/>
+      <c r="N50" s="145"/>
       <c r="O50" s="18"/>
       <c r="P50" s="17"/>
     </row>
@@ -3760,21 +3742,48 @@
     <protectedRange algorithmName="SHA-512" hashValue="NcQe0VjxFnxU9SziGkmWOoYUYoQ0T62vv+WqFE1sowJD2+jDiq1RKEMS6wObDPCk433k/JG1CTU3j62rwNOzdg==" saltValue="OlYFZTFPx5QDCqKlqXj8fw==" spinCount="100000" sqref="I20" name="Range1_2_1_2"/>
   </protectedRanges>
   <mergeCells count="71">
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:K13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:K15"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:I21"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:K19"/>
-    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="J50:N50"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="J46:N46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="J47:N47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="J48:N48"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="J45:N45"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="J49:N49"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="G39:M39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="G40:M40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="G41:M41"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="G36:M36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="G37:M37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="G38:M38"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="G33:M33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="G34:M34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="G35:M35"/>
+    <mergeCell ref="D23:I23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:I25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="G32:M32"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="G30:K30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="G31:M31"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="J3:K3"/>
@@ -3789,48 +3798,21 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="D23:I23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:I25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="G32:M32"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="G30:K30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="G31:M31"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="G33:M33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="G34:M34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="G35:M35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="G36:M36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="G37:M37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="G38:M38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="G39:M39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="G40:M40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="G41:M41"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="J45:N45"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="J49:N49"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="J50:N50"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="J46:N46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="J47:N47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="J48:N48"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:I21"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:K19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:K13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:K15"/>
   </mergeCells>
   <conditionalFormatting sqref="N4">
     <cfRule type="containsText" dxfId="32" priority="81" operator="containsText" text="FAIL">
@@ -4133,31 +4115,31 @@
   <sheetData>
     <row r="2" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B2" s="152" t="s">
-        <v>120</v>
-      </c>
-      <c r="C2" s="123"/>
-      <c r="D2" s="123"/>
+        <v>111</v>
+      </c>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
       <c r="G2" s="4"/>
       <c r="H2" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
@@ -4202,33 +4184,33 @@
     </row>
     <row r="5" spans="1:20" ht="191.25" x14ac:dyDescent="0.2">
       <c r="B5" s="150" t="s">
-        <v>127</v>
-      </c>
-      <c r="C5" s="123"/>
-      <c r="D5" s="123"/>
+        <v>118</v>
+      </c>
+      <c r="C5" s="117"/>
+      <c r="D5" s="117"/>
       <c r="F5" s="10">
         <v>6.1</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="N5" s="2" t="e">
         <f ca="1">_xludf.CONCAT(M5,M6)</f>
@@ -4262,22 +4244,22 @@
       <c r="D6" s="93"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -4289,33 +4271,33 @@
     </row>
     <row r="7" spans="1:20" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B7" s="150" t="s">
-        <v>141</v>
-      </c>
-      <c r="C7" s="123"/>
-      <c r="D7" s="123"/>
+        <v>132</v>
+      </c>
+      <c r="C7" s="117"/>
+      <c r="D7" s="117"/>
       <c r="F7" s="10">
         <v>6.2</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="N7" s="2" t="e">
         <f ca="1">_xludf.CONCAT(M7,M8)</f>
@@ -4345,28 +4327,28 @@
     </row>
     <row r="8" spans="1:20" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B8" s="150" t="s">
-        <v>149</v>
-      </c>
-      <c r="C8" s="123"/>
-      <c r="D8" s="123"/>
+        <v>140</v>
+      </c>
+      <c r="C8" s="117"/>
+      <c r="D8" s="117"/>
       <c r="G8" s="4"/>
       <c r="H8" s="9" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
@@ -4413,55 +4395,55 @@
     </row>
     <row r="13" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B13" s="151"/>
-      <c r="C13" s="123"/>
-      <c r="D13" s="123"/>
+      <c r="C13" s="117"/>
+      <c r="D13" s="117"/>
       <c r="G13" s="10"/>
       <c r="H13" s="4" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="150" t="s">
-        <v>161</v>
-      </c>
-      <c r="C14" s="123"/>
-      <c r="D14" s="123"/>
+        <v>152</v>
+      </c>
+      <c r="C14" s="117"/>
+      <c r="D14" s="117"/>
       <c r="F14" s="10">
         <v>3.1</v>
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="5" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="N14" s="2" t="e">
         <f ca="1">_xludf.CONCAT(M14,M15)</f>
@@ -4491,25 +4473,25 @@
     <row r="15" spans="1:20" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="13"/>
       <c r="G15" s="12" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
@@ -4532,31 +4514,31 @@
     </row>
     <row r="18" spans="2:19" ht="255" x14ac:dyDescent="0.2">
       <c r="B18" s="150" t="s">
-        <v>173</v>
-      </c>
-      <c r="C18" s="123"/>
-      <c r="D18" s="123"/>
+        <v>164</v>
+      </c>
+      <c r="C18" s="117"/>
+      <c r="D18" s="117"/>
       <c r="F18" s="10">
         <v>3.2</v>
       </c>
       <c r="G18" s="10"/>
       <c r="H18" s="5" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="N18" s="4" t="e">
         <f ca="1">_xludf.CONCAT(M18,M19)</f>
@@ -4586,15 +4568,15 @@
     <row r="19" spans="2:19" ht="127.5" x14ac:dyDescent="0.2">
       <c r="G19" s="10"/>
       <c r="H19" s="9" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="M19" s="4"/>
     </row>
@@ -4627,55 +4609,55 @@
     </row>
     <row r="24" spans="2:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="H24" s="10" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="K24" s="10" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="L24" s="10" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="M24" s="10" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="2:19" ht="280.5" x14ac:dyDescent="0.2">
       <c r="B25" s="151" t="s">
-        <v>185</v>
-      </c>
-      <c r="C25" s="123"/>
-      <c r="D25" s="123"/>
+        <v>176</v>
+      </c>
+      <c r="C25" s="117"/>
+      <c r="D25" s="117"/>
       <c r="G25" s="10" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="26" spans="2:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G26" s="10" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -4695,9 +4677,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4916,27 +4901,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D98D897-3D5D-4CF5-A274-8B2E15AE73B2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BB72468-B9EB-412A-8D55-6151E9A308C0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="bd38d267-56bb-4e22-b975-199a06fd69fa"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="d8c712e5-67fc-4595-93cb-a4164dd8eff3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4961,9 +4934,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BB72468-B9EB-412A-8D55-6151E9A308C0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D98D897-3D5D-4CF5-A274-8B2E15AE73B2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="bd38d267-56bb-4e22-b975-199a06fd69fa"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="d8c712e5-67fc-4595-93cb-a4164dd8eff3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>